<commit_message>
Updated timesheet of Stamatina Tounta
</commit_message>
<xml_diff>
--- a/Project_management/ip_sdi_time_sheet_s1095334.xlsx
+++ b/Project_management/ip_sdi_time_sheet_s1095334.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://plusacat-my.sharepoint.com/personal/stamatina_tounta_stud_plus_ac_at/Documents/3rd semester/IP_SDI/4. Project/3. Project management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{70D4A704-C547-4687-9C54-B5A46D362BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3ACF3ACF-378B-44CC-B0CF-BC5064989BC1}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="13_ncr:1_{70D4A704-C547-4687-9C54-B5A46D362BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF4F441A-F11C-4AE5-904D-5EC71419FA78}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="893" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="893" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="October" sheetId="7" r:id="rId1"/>
@@ -22,11 +22,11 @@
     <definedName name="E_satz">#REF!</definedName>
     <definedName name="M_satz">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">December!$A$1:$L$49</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">January!$A$1:$L$47</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">January!$A$1:$L$49</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">November!$A$1:$L$47</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">October!$A$1:$I$48</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">December!$16:$18</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="3">January!$16:$17</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">January!$16:$18</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">November!$16:$17</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">October!$13:$15</definedName>
     <definedName name="S_satz">#REF!</definedName>
@@ -46,6 +46,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="82">
   <si>
     <t>Monthly timesheet for MSc Geoinformatics ip:sdi - 23W856162</t>
   </si>
@@ -64,6 +65,9 @@
     <t>Firstname Lastname</t>
   </si>
   <si>
+    <t>Stamatina Tounta</t>
+  </si>
+  <si>
     <t>Project Acronym</t>
   </si>
   <si>
@@ -71,6 +75,9 @@
   </si>
   <si>
     <t>Project Title</t>
+  </si>
+  <si>
+    <t>Sudan: monitoring migrant movements related to the 2023 conflict</t>
   </si>
   <si>
     <t>TIME</t>
@@ -119,6 +126,9 @@
     <t>3.</t>
   </si>
   <si>
+    <t>Course start</t>
+  </si>
+  <si>
     <t>4.</t>
   </si>
   <si>
@@ -128,6 +138,9 @@
     <t>6.</t>
   </si>
   <si>
+    <t>Project topic brainstorming</t>
+  </si>
+  <si>
     <t>7.</t>
   </si>
   <si>
@@ -146,18 +159,27 @@
     <t>12.</t>
   </si>
   <si>
+    <t xml:space="preserve">Search for data &amp; document resources (WP1) </t>
+  </si>
+  <si>
     <t>13.</t>
   </si>
   <si>
     <t>14.</t>
   </si>
   <si>
+    <t>Create sharepoint &amp; notebook (WP0)</t>
+  </si>
+  <si>
     <t>15.</t>
   </si>
   <si>
     <t>16.</t>
   </si>
   <si>
+    <t>Team meeting: Exchange ideas for project topic (WP1)</t>
+  </si>
+  <si>
     <t>17.</t>
   </si>
   <si>
@@ -173,6 +195,9 @@
     <t>21.</t>
   </si>
   <si>
+    <t>Project brainstorming (WP1)</t>
+  </si>
+  <si>
     <t>22.</t>
   </si>
   <si>
@@ -185,6 +210,9 @@
     <t>25.</t>
   </si>
   <si>
+    <t>Search for geodata (WP1)</t>
+  </si>
+  <si>
     <t>26.</t>
   </si>
   <si>
@@ -200,63 +228,36 @@
     <t>30.</t>
   </si>
   <si>
+    <t>Team meeting:Project management (WP0) &amp; go through data, define variables to analyze, brainstorming for dashboard design (WP1)</t>
+  </si>
+  <si>
     <t>31.</t>
   </si>
   <si>
-    <t>Stamatina Tounta</t>
-  </si>
-  <si>
-    <t>Sudan: monitoring migrant movements related to the 2023 conflict</t>
-  </si>
-  <si>
-    <t>Course start</t>
-  </si>
-  <si>
-    <t>Project topic brainstorming</t>
+    <t>Team meeting:Project management (define WP, tasks etc) (WP0)</t>
+  </si>
+  <si>
+    <t>Team meeting:Project management (define WP, tasks, gantt chart, milestones) (WP0)</t>
+  </si>
+  <si>
+    <t>Research for data preprocessing (WP2)</t>
+  </si>
+  <si>
+    <t>Datasets download (WP1)</t>
+  </si>
+  <si>
+    <t>Team meeting: identify suitable datasets (because of the data inconsistencies) (WP1)</t>
+  </si>
+  <si>
+    <t>Dashboard tutorials</t>
+  </si>
+  <si>
+    <t>Preparing workflow diagram &amp; updating GitLab (WP0)</t>
   </si>
   <si>
     <t>Preparing interim presentation (WP0)</t>
   </si>
   <si>
-    <t>Preparing workflow diagram &amp; updating GitLab (WP0)</t>
-  </si>
-  <si>
-    <t>Team meeting:Project management (define WP, tasks etc) (WP0)</t>
-  </si>
-  <si>
-    <t>Team meeting:Project management (define WP, tasks, gantt chart, milestones) (WP0)</t>
-  </si>
-  <si>
-    <t>Dashboard tutorials</t>
-  </si>
-  <si>
-    <t>Team meeting: identify suitable datasets (because of the data inconsistencies) (WP1)</t>
-  </si>
-  <si>
-    <t>Datasets download (WP1)</t>
-  </si>
-  <si>
-    <t>Team meeting:Project management (WP0) &amp; go through data, define variables to analyze, brainstorming for dashboard design (WP1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search for data &amp; document resources (WP1) </t>
-  </si>
-  <si>
-    <t>Team meeting: Exchange ideas for project topic (WP1)</t>
-  </si>
-  <si>
-    <t>Create sharepoint &amp; notebook (WP0)</t>
-  </si>
-  <si>
-    <t>Search for geodata (WP1)</t>
-  </si>
-  <si>
-    <t>Project brainstorming (WP1)</t>
-  </si>
-  <si>
-    <t>Research for data preprocessing (WP2)</t>
-  </si>
-  <si>
     <t>Team meeting: finalizing interim presentation (WP0)</t>
   </si>
   <si>
@@ -270,6 +271,45 @@
   </si>
   <si>
     <t>GitLab update (WP0)</t>
+  </si>
+  <si>
+    <t>Data preparation - creating one dataset with monthly IDPs updates (WP2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Team meeting: data preparation and integration into the PostGIS DB (changing column names etc), decide on Web services needed for the project (WP 2 &amp; WP 3)/ Creation and publishing of web services in the ArcGIS environment (WP 3) </t>
+  </si>
+  <si>
+    <t>Trying to set up ArcGIS insights &amp; search for tutorials (WP4)</t>
+  </si>
+  <si>
+    <t>Join data, cleaning and integration into the PostGIS database (WP2)</t>
+  </si>
+  <si>
+    <t>Trying to set up ArcGIS insights (WP4), updating GitLab Issues (WP0)</t>
+  </si>
+  <si>
+    <t>Team meeting: Project management (WP0) and ArcGIS Insights walktrhough (WP4)</t>
+  </si>
+  <si>
+    <t>Dashboard brainstorming &amp; ArcGIS Insights tutorials</t>
+  </si>
+  <si>
+    <t>Team meeting: trying to create links in maps (WP4)</t>
+  </si>
+  <si>
+    <t>Testing map links (WP4)</t>
+  </si>
+  <si>
+    <t>ArcGIS Insights tutorials and brainstorming (WP4)</t>
+  </si>
+  <si>
+    <t>Creating linked maps in ArcGIS Insights and trying different methods to join the data (WP4)</t>
+  </si>
+  <si>
+    <t>ArcGIS Insights tutorial for presenting migration data, trying to pre-process our data to be able to create linked maps in ArcGIS Insights (WP2)</t>
+  </si>
+  <si>
+    <t>Project management brainstorming (WP0)</t>
   </si>
 </sst>
 </file>
@@ -742,7 +782,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -832,7 +872,7 @@
     <xf numFmtId="167" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -857,7 +897,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="10" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -928,6 +968,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1342,7 +1391,7 @@
   </sheetPr>
   <dimension ref="A1:AW50"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A27" zoomScale="120" zoomScaleNormal="100" zoomScaleSheetLayoutView="120" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="120" zoomScaleNormal="100" zoomScaleSheetLayoutView="120" workbookViewId="0">
       <selection activeCell="E37" sqref="E37:I37"/>
     </sheetView>
   </sheetViews>
@@ -1459,7 +1508,7 @@
       <c r="B5" s="65"/>
       <c r="C5" s="65"/>
       <c r="D5" s="66" t="s">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="E5" s="67"/>
       <c r="F5" s="67"/>
@@ -1480,12 +1529,12 @@
     </row>
     <row r="7" spans="1:49" s="1" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="70" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" s="70"/>
       <c r="C7" s="70"/>
       <c r="D7" s="71" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E7" s="71"/>
       <c r="F7" s="71"/>
@@ -1506,12 +1555,12 @@
     </row>
     <row r="9" spans="1:49" s="1" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="70" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" s="70"/>
       <c r="C9" s="70"/>
       <c r="D9" s="66" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="E9" s="67"/>
       <c r="F9" s="67"/>
@@ -1533,12 +1582,12 @@
     </row>
     <row r="11" spans="1:49" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B11" s="34"/>
       <c r="C11" s="34"/>
       <c r="D11" s="34" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E11" s="34"/>
       <c r="F11" s="34"/>
@@ -1559,10 +1608,10 @@
     </row>
     <row r="13" spans="1:49" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="47" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C13" s="51"/>
       <c r="D13" s="51"/>
@@ -1575,14 +1624,14 @@
     <row r="14" spans="1:49" s="2" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="48"/>
       <c r="B14" s="53" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C14" s="54"/>
       <c r="D14" s="55" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E14" s="57" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F14" s="58"/>
       <c r="G14" s="58"/>
@@ -1592,10 +1641,10 @@
     <row r="15" spans="1:49" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="49"/>
       <c r="B15" s="21" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D15" s="56"/>
       <c r="E15" s="60"/>
@@ -1606,7 +1655,7 @@
     </row>
     <row r="16" spans="1:49" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="31"/>
@@ -1622,7 +1671,7 @@
     </row>
     <row r="17" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B17" s="30"/>
       <c r="C17" s="31"/>
@@ -1638,7 +1687,7 @@
     </row>
     <row r="18" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B18" s="26"/>
       <c r="C18" s="27"/>
@@ -1647,7 +1696,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="36" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="F18" s="37"/>
       <c r="G18" s="37"/>
@@ -1656,7 +1705,7 @@
     </row>
     <row r="19" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B19" s="26"/>
       <c r="C19" s="27"/>
@@ -1672,7 +1721,7 @@
     </row>
     <row r="20" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B20" s="30"/>
       <c r="C20" s="31"/>
@@ -1688,7 +1737,7 @@
     </row>
     <row r="21" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B21" s="30">
         <v>0.75</v>
@@ -1701,7 +1750,7 @@
         <v>8.333333333333337E-2</v>
       </c>
       <c r="E21" s="39" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="F21" s="40"/>
       <c r="G21" s="40"/>
@@ -1710,7 +1759,7 @@
     </row>
     <row r="22" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B22" s="30"/>
       <c r="C22" s="31"/>
@@ -1726,7 +1775,7 @@
     </row>
     <row r="23" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B23" s="30"/>
       <c r="C23" s="31"/>
@@ -1742,7 +1791,7 @@
     </row>
     <row r="24" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B24" s="30"/>
       <c r="C24" s="31"/>
@@ -1758,7 +1807,7 @@
     </row>
     <row r="25" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B25" s="26"/>
       <c r="C25" s="27"/>
@@ -1774,7 +1823,7 @@
     </row>
     <row r="26" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B26" s="26"/>
       <c r="C26" s="27"/>
@@ -1790,7 +1839,7 @@
     </row>
     <row r="27" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B27" s="30">
         <v>0.72916666666666663</v>
@@ -1803,7 +1852,7 @@
         <v>8.333333333333337E-2</v>
       </c>
       <c r="E27" s="39" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="F27" s="40"/>
       <c r="G27" s="40"/>
@@ -1812,7 +1861,7 @@
     </row>
     <row r="28" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B28" s="30">
         <v>0.75</v>
@@ -1825,7 +1874,7 @@
         <v>8.333333333333337E-2</v>
       </c>
       <c r="E28" s="39" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="F28" s="40"/>
       <c r="G28" s="40"/>
@@ -1834,7 +1883,7 @@
     </row>
     <row r="29" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="29" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B29" s="30">
         <v>0.79166666666666663</v>
@@ -1847,7 +1896,7 @@
         <v>4.1666666666666741E-2</v>
       </c>
       <c r="E29" s="39" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="F29" s="40"/>
       <c r="G29" s="40"/>
@@ -1856,7 +1905,7 @@
     </row>
     <row r="30" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="29" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B30" s="30"/>
       <c r="C30" s="31"/>
@@ -1872,7 +1921,7 @@
     </row>
     <row r="31" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B31" s="30">
         <v>0.70833333333333337</v>
@@ -1885,7 +1934,7 @@
         <v>6.25E-2</v>
       </c>
       <c r="E31" s="39" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="F31" s="40"/>
       <c r="G31" s="40"/>
@@ -1894,7 +1943,7 @@
     </row>
     <row r="32" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B32" s="26"/>
       <c r="C32" s="27"/>
@@ -1910,7 +1959,7 @@
     </row>
     <row r="33" spans="1:13" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B33" s="26"/>
       <c r="C33" s="27"/>
@@ -1926,7 +1975,7 @@
     </row>
     <row r="34" spans="1:13" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B34" s="30"/>
       <c r="C34" s="31"/>
@@ -1942,7 +1991,7 @@
     </row>
     <row r="35" spans="1:13" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B35" s="30"/>
       <c r="C35" s="31"/>
@@ -1958,7 +2007,7 @@
     </row>
     <row r="36" spans="1:13" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="29" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B36" s="30">
         <v>0.6875</v>
@@ -1971,7 +2020,7 @@
         <v>2.083333333333337E-2</v>
       </c>
       <c r="E36" s="39" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="F36" s="40"/>
       <c r="G36" s="40"/>
@@ -1980,7 +2029,7 @@
     </row>
     <row r="37" spans="1:13" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="29" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B37" s="30"/>
       <c r="C37" s="31"/>
@@ -1996,7 +2045,7 @@
     </row>
     <row r="38" spans="1:13" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="29" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B38" s="30"/>
       <c r="C38" s="31"/>
@@ -2012,7 +2061,7 @@
     </row>
     <row r="39" spans="1:13" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B39" s="26"/>
       <c r="C39" s="27"/>
@@ -2028,7 +2077,7 @@
     </row>
     <row r="40" spans="1:13" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B40" s="26">
         <v>0.66666666666666663</v>
@@ -2041,7 +2090,7 @@
         <v>8.333333333333337E-2</v>
       </c>
       <c r="E40" s="36" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="F40" s="37"/>
       <c r="G40" s="37"/>
@@ -2050,7 +2099,7 @@
     </row>
     <row r="41" spans="1:13" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="29" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B41" s="30"/>
       <c r="C41" s="31"/>
@@ -2066,7 +2115,7 @@
     </row>
     <row r="42" spans="1:13" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="29" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B42" s="30"/>
       <c r="C42" s="31"/>
@@ -2082,7 +2131,7 @@
     </row>
     <row r="43" spans="1:13" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="29" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B43" s="30"/>
       <c r="C43" s="31"/>
@@ -2098,7 +2147,7 @@
     </row>
     <row r="44" spans="1:13" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="29" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B44" s="30"/>
       <c r="C44" s="31"/>
@@ -2114,7 +2163,7 @@
     </row>
     <row r="45" spans="1:13" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="29" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B45" s="30">
         <v>0.75</v>
@@ -2127,7 +2176,7 @@
         <v>8.333333333333337E-2</v>
       </c>
       <c r="E45" s="39" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F45" s="40"/>
       <c r="G45" s="40"/>
@@ -2136,7 +2185,7 @@
     </row>
     <row r="46" spans="1:13" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="25" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B46" s="26"/>
       <c r="C46" s="27"/>
@@ -2259,8 +2308,8 @@
   </sheetPr>
   <dimension ref="A1:AR47"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45:I45"/>
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42:I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -2451,7 +2500,7 @@
     </row>
     <row r="11" spans="1:44" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B11" s="34"/>
       <c r="C11" s="34"/>
@@ -2478,10 +2527,10 @@
     </row>
     <row r="13" spans="1:44" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="47" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C13" s="51"/>
       <c r="D13" s="51"/>
@@ -2494,14 +2543,14 @@
     <row r="14" spans="1:44" s="2" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="48"/>
       <c r="B14" s="53" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C14" s="54"/>
       <c r="D14" s="55" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E14" s="57" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F14" s="58"/>
       <c r="G14" s="58"/>
@@ -2511,10 +2560,10 @@
     <row r="15" spans="1:44" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="49"/>
       <c r="B15" s="21" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D15" s="56"/>
       <c r="E15" s="60"/>
@@ -2525,7 +2574,7 @@
     </row>
     <row r="16" spans="1:44" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B16" s="26"/>
       <c r="C16" s="27"/>
@@ -2541,7 +2590,7 @@
     </row>
     <row r="17" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B17" s="30"/>
       <c r="C17" s="31"/>
@@ -2557,7 +2606,7 @@
     </row>
     <row r="18" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B18" s="30">
         <v>0.625</v>
@@ -2570,7 +2619,7 @@
         <v>8.333333333333337E-2</v>
       </c>
       <c r="E18" s="39" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F18" s="40"/>
       <c r="G18" s="40"/>
@@ -2579,7 +2628,7 @@
     </row>
     <row r="19" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B19" s="30"/>
       <c r="C19" s="31"/>
@@ -2595,7 +2644,7 @@
     </row>
     <row r="20" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B20" s="30"/>
       <c r="C20" s="31"/>
@@ -2611,7 +2660,7 @@
     </row>
     <row r="21" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B21" s="30">
         <v>0.75</v>
@@ -2624,7 +2673,7 @@
         <v>8.333333333333337E-2</v>
       </c>
       <c r="E21" s="39" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F21" s="40"/>
       <c r="G21" s="40"/>
@@ -2633,7 +2682,7 @@
     </row>
     <row r="22" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B22" s="26"/>
       <c r="C22" s="27"/>
@@ -2649,7 +2698,7 @@
     </row>
     <row r="23" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B23" s="26"/>
       <c r="C23" s="27"/>
@@ -2665,7 +2714,7 @@
     </row>
     <row r="24" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B24" s="30">
         <v>0.70833333333333337</v>
@@ -2678,7 +2727,7 @@
         <v>6.25E-2</v>
       </c>
       <c r="E24" s="39" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F24" s="40"/>
       <c r="G24" s="40"/>
@@ -2687,7 +2736,7 @@
     </row>
     <row r="25" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B25" s="30"/>
       <c r="C25" s="31"/>
@@ -2703,7 +2752,7 @@
     </row>
     <row r="26" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B26" s="30"/>
       <c r="C26" s="31"/>
@@ -2719,7 +2768,7 @@
     </row>
     <row r="27" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B27" s="30"/>
       <c r="C27" s="31"/>
@@ -2735,7 +2784,7 @@
     </row>
     <row r="28" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B28" s="30">
         <v>0.79166666666666663</v>
@@ -2748,7 +2797,7 @@
         <v>4.1666666666666741E-2</v>
       </c>
       <c r="E28" s="39" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F28" s="40"/>
       <c r="G28" s="40"/>
@@ -2757,7 +2806,7 @@
     </row>
     <row r="29" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B29" s="26"/>
       <c r="C29" s="27"/>
@@ -2773,7 +2822,7 @@
     </row>
     <row r="30" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B30" s="26">
         <v>0.72916666666666663</v>
@@ -2786,7 +2835,7 @@
         <v>8.333333333333337E-2</v>
       </c>
       <c r="E30" s="36" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="F30" s="37"/>
       <c r="G30" s="37"/>
@@ -2795,7 +2844,7 @@
     </row>
     <row r="31" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B31" s="30">
         <v>0.70833333333333337</v>
@@ -2808,7 +2857,7 @@
         <v>4.166666666666663E-2</v>
       </c>
       <c r="E31" s="39" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="F31" s="40"/>
       <c r="G31" s="40"/>
@@ -2817,7 +2866,7 @@
     </row>
     <row r="32" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="29" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B32" s="30"/>
       <c r="C32" s="31"/>
@@ -2833,7 +2882,7 @@
     </row>
     <row r="33" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="29" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B33" s="30"/>
       <c r="C33" s="31"/>
@@ -2849,7 +2898,7 @@
     </row>
     <row r="34" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B34" s="30"/>
       <c r="C34" s="31"/>
@@ -2865,7 +2914,7 @@
     </row>
     <row r="35" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B35" s="30">
         <v>0.70833333333333337</v>
@@ -2878,7 +2927,7 @@
         <v>8.3333333333333259E-2</v>
       </c>
       <c r="E35" s="39" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F35" s="40"/>
       <c r="G35" s="40"/>
@@ -2887,7 +2936,7 @@
     </row>
     <row r="36" spans="1:12" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B36" s="26"/>
       <c r="C36" s="27"/>
@@ -2903,7 +2952,7 @@
     </row>
     <row r="37" spans="1:12" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B37" s="26"/>
       <c r="C37" s="27"/>
@@ -2919,7 +2968,7 @@
     </row>
     <row r="38" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="29" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B38" s="30">
         <v>0.58333333333333337</v>
@@ -2932,7 +2981,7 @@
         <v>4.166666666666663E-2</v>
       </c>
       <c r="E38" s="39" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="F38" s="40"/>
       <c r="G38" s="40"/>
@@ -2941,7 +2990,7 @@
     </row>
     <row r="39" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="29" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B39" s="30"/>
       <c r="C39" s="31"/>
@@ -2957,7 +3006,7 @@
     </row>
     <row r="40" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="29" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B40" s="30">
         <v>0.54166666666666663</v>
@@ -2970,7 +3019,7 @@
         <v>4.1666666666666741E-2</v>
       </c>
       <c r="E40" s="39" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="F40" s="40"/>
       <c r="G40" s="40"/>
@@ -2979,7 +3028,7 @@
     </row>
     <row r="41" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="29" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B41" s="30"/>
       <c r="C41" s="31"/>
@@ -2995,7 +3044,7 @@
     </row>
     <row r="42" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="29" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B42" s="30">
         <v>0.70833333333333337</v>
@@ -3017,7 +3066,7 @@
     </row>
     <row r="43" spans="1:12" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B43" s="26"/>
       <c r="C43" s="27"/>
@@ -3033,7 +3082,7 @@
     </row>
     <row r="44" spans="1:12" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B44" s="26">
         <v>0.73958333333333337</v>
@@ -3055,7 +3104,7 @@
     </row>
     <row r="45" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="29" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B45" s="30">
         <v>0.39583333333333331</v>
@@ -3170,8 +3219,8 @@
   </sheetPr>
   <dimension ref="A1:AM49"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="120" zoomScaleNormal="100" zoomScaleSheetLayoutView="120" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18:I18"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47:I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -3356,7 +3405,7 @@
     </row>
     <row r="11" spans="1:39" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B11" s="34"/>
       <c r="C11" s="34"/>
@@ -3383,10 +3432,10 @@
     </row>
     <row r="13" spans="1:39" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="47" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C13" s="51"/>
       <c r="D13" s="51"/>
@@ -3399,14 +3448,14 @@
     <row r="14" spans="1:39" s="2" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="48"/>
       <c r="B14" s="53" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C14" s="54"/>
       <c r="D14" s="55" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E14" s="57" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F14" s="58"/>
       <c r="G14" s="58"/>
@@ -3416,10 +3465,10 @@
     <row r="15" spans="1:39" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="49"/>
       <c r="B15" s="21" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D15" s="56"/>
       <c r="E15" s="60"/>
@@ -3430,7 +3479,7 @@
     </row>
     <row r="16" spans="1:39" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="77" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B16" s="30">
         <v>0.45833333333333331</v>
@@ -3439,7 +3488,7 @@
         <v>0.5</v>
       </c>
       <c r="D16" s="31">
-        <f>C16-B16</f>
+        <f t="shared" ref="D16:D47" si="0">C16-B16</f>
         <v>4.1666666666666685E-2</v>
       </c>
       <c r="E16" s="39" t="s">
@@ -3459,7 +3508,7 @@
         <v>0.75</v>
       </c>
       <c r="D17" s="31">
-        <f>C17-B17</f>
+        <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
       <c r="E17" s="39" t="s">
@@ -3472,12 +3521,12 @@
     </row>
     <row r="18" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B18" s="30"/>
       <c r="C18" s="31"/>
       <c r="D18" s="31">
-        <f>C18-B18</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E18" s="39"/>
@@ -3488,15 +3537,21 @@
     </row>
     <row r="19" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="31"/>
+        <v>19</v>
+      </c>
+      <c r="B19" s="30">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C19" s="31">
+        <v>0.875</v>
+      </c>
       <c r="D19" s="31">
-        <f>C19-B19</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="39"/>
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E19" s="39" t="s">
+        <v>69</v>
+      </c>
       <c r="F19" s="40"/>
       <c r="G19" s="40"/>
       <c r="H19" s="40"/>
@@ -3504,12 +3559,12 @@
     </row>
     <row r="20" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B20" s="30"/>
       <c r="C20" s="31"/>
       <c r="D20" s="31">
-        <f>C20-B20</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E20" s="39"/>
@@ -3520,12 +3575,12 @@
     </row>
     <row r="21" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B21" s="26"/>
       <c r="C21" s="27"/>
       <c r="D21" s="27">
-        <f>C21-B21</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E21" s="36"/>
@@ -3536,12 +3591,12 @@
     </row>
     <row r="22" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B22" s="26"/>
       <c r="C22" s="27"/>
       <c r="D22" s="27">
-        <f>C22-B22</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E22" s="36"/>
@@ -3552,12 +3607,12 @@
     </row>
     <row r="23" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B23" s="30"/>
       <c r="C23" s="31"/>
       <c r="D23" s="31">
-        <f>C23-B23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E23" s="39"/>
@@ -3568,12 +3623,12 @@
     </row>
     <row r="24" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B24" s="30"/>
       <c r="C24" s="31"/>
       <c r="D24" s="31">
-        <f>C24-B24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E24" s="39"/>
@@ -3584,12 +3639,12 @@
     </row>
     <row r="25" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B25" s="30"/>
       <c r="C25" s="31"/>
       <c r="D25" s="31">
-        <f>C25-B25</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E25" s="39"/>
@@ -3600,12 +3655,12 @@
     </row>
     <row r="26" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B26" s="30"/>
       <c r="C26" s="31"/>
       <c r="D26" s="31">
-        <f>C26-B26</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E26" s="39"/>
@@ -3616,12 +3671,12 @@
     </row>
     <row r="27" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B27" s="30"/>
       <c r="C27" s="31"/>
       <c r="D27" s="31">
-        <f>C27-B27</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E27" s="39"/>
@@ -3632,12 +3687,12 @@
     </row>
     <row r="28" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B28" s="26"/>
       <c r="C28" s="27"/>
       <c r="D28" s="27">
-        <f>C28-B28</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E28" s="36"/>
@@ -3648,12 +3703,12 @@
     </row>
     <row r="29" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B29" s="26"/>
       <c r="C29" s="27"/>
       <c r="D29" s="27">
-        <f>C29-B29</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E29" s="36"/>
@@ -3664,12 +3719,12 @@
     </row>
     <row r="30" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="29" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B30" s="30"/>
       <c r="C30" s="31"/>
       <c r="D30" s="31">
-        <f>C30-B30</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E30" s="39"/>
@@ -3680,12 +3735,12 @@
     </row>
     <row r="31" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B31" s="30"/>
       <c r="C31" s="31"/>
       <c r="D31" s="31">
-        <f>C31-B31</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E31" s="39"/>
@@ -3696,12 +3751,12 @@
     </row>
     <row r="32" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="29" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B32" s="30"/>
       <c r="C32" s="31"/>
       <c r="D32" s="31">
-        <f>C32-B32</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E32" s="39"/>
@@ -3712,15 +3767,21 @@
     </row>
     <row r="33" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="30"/>
-      <c r="C33" s="31"/>
+        <v>38</v>
+      </c>
+      <c r="B33" s="30">
+        <v>0.75</v>
+      </c>
+      <c r="C33" s="31">
+        <v>0.83333333333333337</v>
+      </c>
       <c r="D33" s="31">
-        <f>C33-B33</f>
-        <v>0</v>
-      </c>
-      <c r="E33" s="39"/>
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E33" s="39" t="s">
+        <v>72</v>
+      </c>
       <c r="F33" s="40"/>
       <c r="G33" s="40"/>
       <c r="H33" s="40"/>
@@ -3728,12 +3789,12 @@
     </row>
     <row r="34" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B34" s="30"/>
       <c r="C34" s="31"/>
       <c r="D34" s="31">
-        <f>C34-B34</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E34" s="39"/>
@@ -3744,12 +3805,12 @@
     </row>
     <row r="35" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B35" s="26"/>
       <c r="C35" s="27"/>
       <c r="D35" s="27">
-        <f>C35-B35</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E35" s="36"/>
@@ -3760,15 +3821,21 @@
     </row>
     <row r="36" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" s="26"/>
-      <c r="C36" s="27"/>
+        <v>41</v>
+      </c>
+      <c r="B36" s="26">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C36" s="27">
+        <v>0.75</v>
+      </c>
       <c r="D36" s="27">
-        <f>C36-B36</f>
-        <v>0</v>
-      </c>
-      <c r="E36" s="36"/>
+        <f t="shared" si="0"/>
+        <v>0.16666666666666663</v>
+      </c>
+      <c r="E36" s="36" t="s">
+        <v>70</v>
+      </c>
       <c r="F36" s="37"/>
       <c r="G36" s="37"/>
       <c r="H36" s="37"/>
@@ -3776,15 +3843,21 @@
     </row>
     <row r="37" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" s="30"/>
-      <c r="C37" s="31"/>
+        <v>42</v>
+      </c>
+      <c r="B37" s="30">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C37" s="31">
+        <v>0.75</v>
+      </c>
       <c r="D37" s="31">
-        <f>C37-B37</f>
-        <v>0</v>
-      </c>
-      <c r="E37" s="39"/>
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E37" s="39" t="s">
+        <v>71</v>
+      </c>
       <c r="F37" s="40"/>
       <c r="G37" s="40"/>
       <c r="H37" s="40"/>
@@ -3792,15 +3865,21 @@
     </row>
     <row r="38" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38" s="30"/>
-      <c r="C38" s="31"/>
+        <v>44</v>
+      </c>
+      <c r="B38" s="30">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C38" s="31">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="D38" s="31">
-        <f>C38-B38</f>
-        <v>0</v>
-      </c>
-      <c r="E38" s="39"/>
+        <f t="shared" si="0"/>
+        <v>8.3333333333333259E-2</v>
+      </c>
+      <c r="E38" s="39" t="s">
+        <v>73</v>
+      </c>
       <c r="F38" s="40"/>
       <c r="G38" s="40"/>
       <c r="H38" s="40"/>
@@ -3808,12 +3887,12 @@
     </row>
     <row r="39" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="29" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B39" s="30"/>
       <c r="C39" s="31"/>
       <c r="D39" s="31">
-        <f>C39-B39</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E39" s="39"/>
@@ -3824,12 +3903,12 @@
     </row>
     <row r="40" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="29" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B40" s="30"/>
       <c r="C40" s="31"/>
       <c r="D40" s="31">
-        <f>C40-B40</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E40" s="39"/>
@@ -3840,12 +3919,12 @@
     </row>
     <row r="41" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="29" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="B41" s="30"/>
       <c r="C41" s="31"/>
       <c r="D41" s="31">
-        <f>C41-B41</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E41" s="39"/>
@@ -3856,12 +3935,12 @@
     </row>
     <row r="42" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="25" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B42" s="26"/>
       <c r="C42" s="27"/>
       <c r="D42" s="27">
-        <f>C42-B42</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E42" s="36"/>
@@ -3872,12 +3951,12 @@
     </row>
     <row r="43" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B43" s="26"/>
       <c r="C43" s="27"/>
       <c r="D43" s="27">
-        <f>C43-B43</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E43" s="36"/>
@@ -3888,12 +3967,12 @@
     </row>
     <row r="44" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="29" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B44" s="30"/>
       <c r="C44" s="31"/>
       <c r="D44" s="31">
-        <f>C44-B44</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E44" s="39"/>
@@ -3904,15 +3983,21 @@
     </row>
     <row r="45" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B45" s="30"/>
-      <c r="C45" s="31"/>
+        <v>52</v>
+      </c>
+      <c r="B45" s="30">
+        <v>0.5625</v>
+      </c>
+      <c r="C45" s="31">
+        <v>0.60416666666666663</v>
+      </c>
       <c r="D45" s="31">
-        <f>C45-B45</f>
-        <v>0</v>
-      </c>
-      <c r="E45" s="39"/>
+        <f t="shared" si="0"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E45" s="39" t="s">
+        <v>74</v>
+      </c>
       <c r="F45" s="40"/>
       <c r="G45" s="40"/>
       <c r="H45" s="40"/>
@@ -3920,15 +4005,21 @@
     </row>
     <row r="46" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="29" t="s">
-        <v>44</v>
-      </c>
-      <c r="B46" s="30"/>
-      <c r="C46" s="31"/>
+        <v>53</v>
+      </c>
+      <c r="B46" s="30">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C46" s="31">
+        <v>0.54166666666666663</v>
+      </c>
       <c r="D46" s="31">
-        <f>C46-B46</f>
-        <v>0</v>
-      </c>
-      <c r="E46" s="39"/>
+        <f t="shared" si="0"/>
+        <v>8.3333333333333315E-2</v>
+      </c>
+      <c r="E46" s="39" t="s">
+        <v>75</v>
+      </c>
       <c r="F46" s="40"/>
       <c r="G46" s="40"/>
       <c r="H46" s="40"/>
@@ -3936,12 +4027,12 @@
     </row>
     <row r="47" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="29" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B47" s="30"/>
       <c r="C47" s="31"/>
       <c r="D47" s="31">
-        <f>C47-B47</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E47" s="39"/>
@@ -3956,7 +4047,7 @@
       <c r="C48" s="43"/>
       <c r="D48" s="23">
         <f>SUM(D16:D47)</f>
-        <v>0.12500000000000006</v>
+        <v>0.75</v>
       </c>
       <c r="E48" s="44"/>
       <c r="F48" s="44"/>
@@ -3980,9 +4071,9 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="E16:I16"/>
     <mergeCell ref="A6:I6"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:I2"/>
@@ -3990,36 +4081,33 @@
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="D5:H5"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="E17:H17"/>
     <mergeCell ref="E19:I19"/>
     <mergeCell ref="E20:I20"/>
     <mergeCell ref="E18:I18"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="E29:I29"/>
     <mergeCell ref="E24:I24"/>
     <mergeCell ref="E25:I25"/>
     <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E33:I33"/>
+    <mergeCell ref="E34:I34"/>
+    <mergeCell ref="E35:I35"/>
     <mergeCell ref="E30:I30"/>
     <mergeCell ref="E31:I31"/>
     <mergeCell ref="E32:I32"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="E39:I39"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="E41:I41"/>
     <mergeCell ref="E36:I36"/>
     <mergeCell ref="E37:I37"/>
     <mergeCell ref="E38:I38"/>
-    <mergeCell ref="E33:I33"/>
-    <mergeCell ref="E34:I34"/>
-    <mergeCell ref="E35:I35"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="E44:I44"/>
-    <mergeCell ref="E39:I39"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="E41:I41"/>
     <mergeCell ref="E48:I48"/>
     <mergeCell ref="E45:I45"/>
     <mergeCell ref="E46:I46"/>
@@ -4033,6 +4121,9 @@
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:I15"/>
     <mergeCell ref="A9:C9"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="E44:I44"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.44" right="0.03" top="0.02" bottom="0.03" header="0.19685039370078741" footer="0.19685039370078741"/>
@@ -4046,10 +4137,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AM47"/>
+  <dimension ref="A1:AM49"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="120" zoomScaleNormal="100" zoomScaleSheetLayoutView="120" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:H5"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24:I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -4234,7 +4325,7 @@
     </row>
     <row r="11" spans="1:39" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B11" s="34"/>
       <c r="C11" s="34"/>
@@ -4261,10 +4352,10 @@
     </row>
     <row r="13" spans="1:39" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="47" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C13" s="51"/>
       <c r="D13" s="51"/>
@@ -4277,14 +4368,14 @@
     <row r="14" spans="1:39" s="2" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="48"/>
       <c r="B14" s="53" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C14" s="54"/>
       <c r="D14" s="55" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E14" s="57" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F14" s="58"/>
       <c r="G14" s="58"/>
@@ -4294,10 +4385,10 @@
     <row r="15" spans="1:39" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="49"/>
       <c r="B15" s="21" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D15" s="56"/>
       <c r="E15" s="60"/>
@@ -4308,7 +4399,7 @@
     </row>
     <row r="16" spans="1:39" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B16" s="30"/>
       <c r="C16" s="31"/>
@@ -4322,81 +4413,101 @@
       <c r="H16" s="40"/>
       <c r="I16" s="41"/>
     </row>
-    <row r="17" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27">
-        <f t="shared" ref="D17:D45" si="0">C17-B17</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="38"/>
+    <row r="17" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A17" s="79" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="30">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C17" s="31">
+        <v>0.625</v>
+      </c>
+      <c r="D17" s="31">
+        <f>C17-B17</f>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="41"/>
     </row>
     <row r="18" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="27"/>
+      <c r="A18" s="80"/>
+      <c r="B18" s="26">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C18" s="27">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="D18" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E18" s="36"/>
+        <f t="shared" ref="D18:D47" si="0">C18-B18</f>
+        <v>8.3333333333333259E-2</v>
+      </c>
+      <c r="E18" s="36" t="s">
+        <v>76</v>
+      </c>
       <c r="F18" s="37"/>
       <c r="G18" s="37"/>
       <c r="H18" s="37"/>
       <c r="I18" s="38"/>
     </row>
-    <row r="19" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E19" s="39"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="41"/>
-    </row>
-    <row r="20" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
+    <row r="19" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A19" s="81"/>
+      <c r="B19" s="26">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C19" s="27">
+        <v>0.875</v>
+      </c>
+      <c r="D19" s="27">
+        <f t="shared" si="0"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="E19" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="38"/>
+    </row>
+    <row r="20" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="30"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E20" s="39"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="41"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="36"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="38"/>
     </row>
     <row r="21" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="31"/>
+        <v>21</v>
+      </c>
+      <c r="B21" s="30">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C21" s="31">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="D21" s="31">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E21" s="39"/>
+        <v>0.25</v>
+      </c>
+      <c r="E21" s="39" t="s">
+        <v>80</v>
+      </c>
       <c r="F21" s="40"/>
       <c r="G21" s="40"/>
       <c r="H21" s="40"/>
@@ -4404,15 +4515,21 @@
     </row>
     <row r="22" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="30"/>
-      <c r="C22" s="31"/>
+        <v>22</v>
+      </c>
+      <c r="B22" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="C22" s="31">
+        <v>0.64583333333333337</v>
+      </c>
       <c r="D22" s="31">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E22" s="39"/>
+        <v>0.14583333333333337</v>
+      </c>
+      <c r="E22" s="39" t="s">
+        <v>79</v>
+      </c>
       <c r="F22" s="40"/>
       <c r="G22" s="40"/>
       <c r="H22" s="40"/>
@@ -4420,87 +4537,93 @@
     </row>
     <row r="23" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="31"/>
+        <v>23</v>
+      </c>
+      <c r="B23" s="30">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C23" s="31">
+        <v>0.83333333333333337</v>
+      </c>
       <c r="D23" s="31">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E23" s="39"/>
+        <v>4.1666666666666741E-2</v>
+      </c>
+      <c r="E23" s="39" t="s">
+        <v>81</v>
+      </c>
       <c r="F23" s="40"/>
       <c r="G23" s="40"/>
       <c r="H23" s="40"/>
       <c r="I23" s="41"/>
     </row>
-    <row r="24" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="26"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E24" s="36"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="38"/>
-    </row>
-    <row r="25" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="26"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E25" s="36"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="38"/>
-    </row>
-    <row r="26" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A26" s="29" t="s">
+    <row r="24" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A24" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="30"/>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E26" s="39"/>
-      <c r="F26" s="40"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="41"/>
-    </row>
-    <row r="27" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
+      <c r="B24" s="30"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E24" s="39"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="41"/>
+    </row>
+    <row r="25" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A25" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E27" s="39"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="41"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E25" s="39"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="41"/>
+    </row>
+    <row r="26" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A26" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="26"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E26" s="36"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="38"/>
+    </row>
+    <row r="27" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A27" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="26"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E27" s="36"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="38"/>
     </row>
     <row r="28" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B28" s="30"/>
       <c r="C28" s="31"/>
@@ -4516,7 +4639,7 @@
     </row>
     <row r="29" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="29" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B29" s="30"/>
       <c r="C29" s="31"/>
@@ -4532,7 +4655,7 @@
     </row>
     <row r="30" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="29" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B30" s="30"/>
       <c r="C30" s="31"/>
@@ -4546,73 +4669,73 @@
       <c r="H30" s="40"/>
       <c r="I30" s="41"/>
     </row>
-    <row r="31" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A31" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="26"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E31" s="36"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="38"/>
-    </row>
-    <row r="32" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" s="26"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E32" s="36"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="37"/>
-      <c r="H32" s="37"/>
-      <c r="I32" s="38"/>
-    </row>
-    <row r="33" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A33" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="30"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E33" s="39"/>
-      <c r="F33" s="40"/>
-      <c r="G33" s="40"/>
-      <c r="H33" s="40"/>
-      <c r="I33" s="41"/>
-    </row>
-    <row r="34" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A34" s="29" t="s">
+    <row r="31" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A31" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="30"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E34" s="39"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="41"/>
-    </row>
-    <row r="35" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B31" s="30"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E31" s="39"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="41"/>
+    </row>
+    <row r="32" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A32" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="30"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E32" s="39"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="40"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="41"/>
+    </row>
+    <row r="33" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A33" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="26"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E33" s="36"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="38"/>
+    </row>
+    <row r="34" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A34" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="26"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E34" s="36"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="38"/>
+    </row>
+    <row r="35" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B35" s="30"/>
       <c r="C35" s="31"/>
@@ -4626,9 +4749,9 @@
       <c r="H35" s="40"/>
       <c r="I35" s="41"/>
     </row>
-    <row r="36" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="29" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B36" s="30"/>
       <c r="C36" s="31"/>
@@ -4642,9 +4765,9 @@
       <c r="H36" s="40"/>
       <c r="I36" s="41"/>
     </row>
-    <row r="37" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="29" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B37" s="30"/>
       <c r="C37" s="31"/>
@@ -4658,73 +4781,73 @@
       <c r="H37" s="40"/>
       <c r="I37" s="41"/>
     </row>
-    <row r="38" spans="1:12" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A38" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" s="26"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E38" s="36"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="37"/>
-      <c r="H38" s="37"/>
-      <c r="I38" s="38"/>
-    </row>
-    <row r="39" spans="1:12" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A39" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" s="26"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E39" s="36"/>
-      <c r="F39" s="37"/>
-      <c r="G39" s="37"/>
-      <c r="H39" s="37"/>
-      <c r="I39" s="38"/>
-    </row>
-    <row r="40" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A40" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B40" s="30"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E40" s="39"/>
-      <c r="F40" s="40"/>
-      <c r="G40" s="40"/>
-      <c r="H40" s="40"/>
-      <c r="I40" s="41"/>
-    </row>
-    <row r="41" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A41" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="B41" s="30"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E41" s="39"/>
-      <c r="F41" s="40"/>
-      <c r="G41" s="40"/>
-      <c r="H41" s="40"/>
-      <c r="I41" s="41"/>
-    </row>
-    <row r="42" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A38" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="30"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E38" s="39"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="40"/>
+      <c r="H38" s="40"/>
+      <c r="I38" s="41"/>
+    </row>
+    <row r="39" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A39" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="30"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E39" s="39"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="40"/>
+      <c r="H39" s="40"/>
+      <c r="I39" s="41"/>
+    </row>
+    <row r="40" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A40" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="26"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E40" s="36"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="38"/>
+    </row>
+    <row r="41" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A41" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="26"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E41" s="36"/>
+      <c r="F41" s="37"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="38"/>
+    </row>
+    <row r="42" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="29" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B42" s="30"/>
       <c r="C42" s="31"/>
@@ -4738,9 +4861,9 @@
       <c r="H42" s="40"/>
       <c r="I42" s="41"/>
     </row>
-    <row r="43" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="29" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B43" s="30"/>
       <c r="C43" s="31"/>
@@ -4754,9 +4877,9 @@
       <c r="H43" s="40"/>
       <c r="I43" s="41"/>
     </row>
-    <row r="44" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="29" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B44" s="30"/>
       <c r="C44" s="31"/>
@@ -4770,52 +4893,84 @@
       <c r="H44" s="40"/>
       <c r="I44" s="41"/>
     </row>
-    <row r="45" spans="1:12" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A45" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="B45" s="26"/>
-      <c r="C45" s="27"/>
-      <c r="D45" s="27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E45" s="36"/>
-      <c r="F45" s="37"/>
-      <c r="G45" s="37"/>
-      <c r="H45" s="37"/>
-      <c r="I45" s="38"/>
-    </row>
-    <row r="46" spans="1:12" s="24" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A46" s="42"/>
-      <c r="B46" s="43"/>
-      <c r="C46" s="43"/>
-      <c r="D46" s="23">
-        <f>SUM(D16:D45)</f>
-        <v>0</v>
-      </c>
-      <c r="E46" s="44"/>
-      <c r="F46" s="44"/>
-      <c r="G46" s="44"/>
-      <c r="H46" s="44"/>
-      <c r="I46" s="45"/>
-    </row>
-    <row r="47" spans="1:12" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="18"/>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
-      <c r="I47" s="15"/>
-      <c r="J47" s="9"/>
-      <c r="K47" s="9"/>
-      <c r="L47" s="9"/>
+    <row r="45" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A45" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="30"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E45" s="39"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="40"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="41"/>
+    </row>
+    <row r="46" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A46" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" s="30"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E46" s="39"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="40"/>
+      <c r="H46" s="40"/>
+      <c r="I46" s="41"/>
+    </row>
+    <row r="47" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A47" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47" s="26"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E47" s="36"/>
+      <c r="F47" s="37"/>
+      <c r="G47" s="37"/>
+      <c r="H47" s="37"/>
+      <c r="I47" s="38"/>
+    </row>
+    <row r="48" spans="1:9" s="24" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A48" s="42"/>
+      <c r="B48" s="43"/>
+      <c r="C48" s="43"/>
+      <c r="D48" s="23">
+        <f>SUM(D16:D47)</f>
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E48" s="44"/>
+      <c r="F48" s="44"/>
+      <c r="G48" s="44"/>
+      <c r="H48" s="44"/>
+      <c r="I48" s="45"/>
+    </row>
+    <row r="49" spans="1:12" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="18"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="9"/>
+      <c r="K49" s="9"/>
+      <c r="L49" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="50">
+  <mergeCells count="53">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:H3"/>
@@ -4834,11 +4989,11 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:I15"/>
-    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E39:I39"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="E29:I29"/>
     <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E17:I17"/>
     <mergeCell ref="E18:I18"/>
-    <mergeCell ref="E19:I19"/>
     <mergeCell ref="E20:I20"/>
     <mergeCell ref="E21:I21"/>
     <mergeCell ref="E22:I22"/>
@@ -4846,30 +5001,33 @@
     <mergeCell ref="E24:I24"/>
     <mergeCell ref="E25:I25"/>
     <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E39:I39"/>
+    <mergeCell ref="E27:I27"/>
     <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E29:I29"/>
-    <mergeCell ref="E30:I30"/>
-    <mergeCell ref="E31:I31"/>
-    <mergeCell ref="E32:I32"/>
-    <mergeCell ref="E33:I33"/>
     <mergeCell ref="E34:I34"/>
     <mergeCell ref="E35:I35"/>
     <mergeCell ref="E36:I36"/>
     <mergeCell ref="E37:I37"/>
     <mergeCell ref="E38:I38"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="E46:I46"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="E41:I41"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="E19:I19"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="E48:I48"/>
     <mergeCell ref="E42:I42"/>
     <mergeCell ref="E43:I43"/>
     <mergeCell ref="E44:I44"/>
     <mergeCell ref="E45:I45"/>
+    <mergeCell ref="E46:I46"/>
+    <mergeCell ref="E47:I47"/>
+    <mergeCell ref="E41:I41"/>
+    <mergeCell ref="E30:I30"/>
+    <mergeCell ref="E31:I31"/>
+    <mergeCell ref="E32:I32"/>
+    <mergeCell ref="E33:I33"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.44" right="0.03" top="0.02" bottom="0.03" header="0.19685039370078741" footer="0.19685039370078741"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="95" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Upload most recent timesheet.
</commit_message>
<xml_diff>
--- a/Project_management/ip_sdi_time_sheet_s1095334.xlsx
+++ b/Project_management/ip_sdi_time_sheet_s1095334.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://plusacat-my.sharepoint.com/personal/stamatina_tounta_stud_plus_ac_at/Documents/3rd semester/IP_SDI/4. Project/3. Project management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="13_ncr:1_{70D4A704-C547-4687-9C54-B5A46D362BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF4F441A-F11C-4AE5-904D-5EC71419FA78}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="13_ncr:1_{70D4A704-C547-4687-9C54-B5A46D362BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01B03708-8C5C-45E0-B7A6-48E6022678F6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="893" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="893" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="October" sheetId="7" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="91">
   <si>
     <t>Monthly timesheet for MSc Geoinformatics ip:sdi - 23W856162</t>
   </si>
@@ -276,15 +276,15 @@
     <t>Data preparation - creating one dataset with monthly IDPs updates (WP2)</t>
   </si>
   <si>
+    <t>Join data, cleaning and integration into the PostGIS database (WP2)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Team meeting: data preparation and integration into the PostGIS DB (changing column names etc), decide on Web services needed for the project (WP 2 &amp; WP 3)/ Creation and publishing of web services in the ArcGIS environment (WP 3) </t>
   </si>
   <si>
     <t>Trying to set up ArcGIS insights &amp; search for tutorials (WP4)</t>
   </si>
   <si>
-    <t>Join data, cleaning and integration into the PostGIS database (WP2)</t>
-  </si>
-  <si>
     <t>Trying to set up ArcGIS insights (WP4), updating GitLab Issues (WP0)</t>
   </si>
   <si>
@@ -294,22 +294,49 @@
     <t>Dashboard brainstorming &amp; ArcGIS Insights tutorials</t>
   </si>
   <si>
+    <t>ArcGIS Insights tutorials and brainstorming (WP4)</t>
+  </si>
+  <si>
     <t>Team meeting: trying to create links in maps (WP4)</t>
   </si>
   <si>
     <t>Testing map links (WP4)</t>
   </si>
   <si>
-    <t>ArcGIS Insights tutorials and brainstorming (WP4)</t>
+    <t>ArcGIS Insights tutorial for presenting migration data, trying to pre-process our data to be able to create linked maps in ArcGIS Insights (WP2)</t>
   </si>
   <si>
     <t>Creating linked maps in ArcGIS Insights and trying different methods to join the data (WP4)</t>
   </si>
   <si>
-    <t>ArcGIS Insights tutorial for presenting migration data, trying to pre-process our data to be able to create linked maps in ArcGIS Insights (WP2)</t>
-  </si>
-  <si>
     <t>Project management brainstorming (WP0)</t>
+  </si>
+  <si>
+    <t>Trying different methods to join the data (WP2)</t>
+  </si>
+  <si>
+    <t>Team meeting: Trying different methods to join the data (WP2) and creating linked maps in ArcInsights (WP4)</t>
+  </si>
+  <si>
+    <t>Re-publishing web services (WP3)</t>
+  </si>
+  <si>
+    <t>Team meeting: metadata creation for our point layer (WP2)</t>
+  </si>
+  <si>
+    <t>Team meeting: finish metadata creation for our point layer &amp; create metadata for our admin boundaries layer (WP2)/ Updating GitLab (WP0)</t>
+  </si>
+  <si>
+    <t>Team meeting: ArcGIS Insights creation of final dashboard (WP4)</t>
+  </si>
+  <si>
+    <t>Preparing final presentation (WP0)</t>
+  </si>
+  <si>
+    <t>Team work: Publishing our final web services in ArcGIS Server/Geoportal (WP3) and publishing metadata to Geonetwork (WP2)</t>
+  </si>
+  <si>
+    <t>Team meeting: finalizing ArcGIS Insights (WP4) and final presentation (WP0)/ preparing for the presentation (WP0)</t>
   </si>
 </sst>
 </file>
@@ -845,35 +872,46 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -922,48 +960,37 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1066,9 +1093,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1106,9 +1133,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1141,26 +1168,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1193,26 +1203,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1391,7 +1384,7 @@
   </sheetPr>
   <dimension ref="A1:AW50"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="120" zoomScaleNormal="100" zoomScaleSheetLayoutView="120" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A26" zoomScale="120" zoomScaleNormal="100" zoomScaleSheetLayoutView="120" workbookViewId="0">
       <selection activeCell="E37" sqref="E37:I37"/>
     </sheetView>
   </sheetViews>
@@ -1412,17 +1405,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:49" s="6" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
+      <c r="A1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -1465,120 +1458,120 @@
       <c r="AW1" s="1"/>
     </row>
     <row r="2" spans="1:49" s="1" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="73"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
     </row>
     <row r="3" spans="1:49" s="7" customFormat="1" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
       <c r="I3" s="14"/>
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
     </row>
     <row r="4" spans="1:49" s="1" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="75"/>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:49" s="1" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="65"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="66" t="s">
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="68"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="46"/>
       <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:49" s="1" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="69"/>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="69"/>
-      <c r="H6" s="69"/>
-      <c r="I6" s="69"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
     </row>
     <row r="7" spans="1:49" s="1" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="70" t="s">
+      <c r="A7" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="71" t="s">
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
       <c r="I7" s="15"/>
     </row>
     <row r="8" spans="1:49" s="1" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="76"/>
-      <c r="B8" s="76"/>
-      <c r="C8" s="76"/>
-      <c r="D8" s="76"/>
-      <c r="E8" s="76"/>
-      <c r="F8" s="76"/>
-      <c r="G8" s="76"/>
-      <c r="H8" s="76"/>
-      <c r="I8" s="76"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
     </row>
     <row r="9" spans="1:49" s="1" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="70" t="s">
+      <c r="A9" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="70"/>
-      <c r="C9" s="70"/>
-      <c r="D9" s="66" t="s">
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="68"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="46"/>
       <c r="I9" s="15"/>
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:49" s="1" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="63"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="63"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
     </row>
     <row r="11" spans="1:49" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
@@ -1607,51 +1600,51 @@
       <c r="I12" s="16"/>
     </row>
     <row r="13" spans="1:49" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="52"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="55"/>
     </row>
     <row r="14" spans="1:49" s="2" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="48"/>
-      <c r="B14" s="53" t="s">
+      <c r="A14" s="51"/>
+      <c r="B14" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="54"/>
-      <c r="D14" s="55" t="s">
+      <c r="C14" s="57"/>
+      <c r="D14" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="57" t="s">
+      <c r="E14" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="58"/>
-      <c r="G14" s="58"/>
-      <c r="H14" s="58"/>
-      <c r="I14" s="59"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="62"/>
     </row>
     <row r="15" spans="1:49" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="49"/>
+      <c r="A15" s="52"/>
       <c r="B15" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="56"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
-      <c r="H15" s="61"/>
-      <c r="I15" s="62"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="64"/>
+      <c r="I15" s="65"/>
     </row>
     <row r="16" spans="1:49" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
@@ -1663,11 +1656,11 @@
         <f>C16-B16</f>
         <v>0</v>
       </c>
-      <c r="E16" s="46"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="41"/>
+      <c r="E16" s="72"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="70"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="71"/>
     </row>
     <row r="17" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
@@ -1679,11 +1672,11 @@
         <f t="shared" ref="D17:D46" si="0">C17-B17</f>
         <v>0</v>
       </c>
-      <c r="E17" s="39"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="41"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="70"/>
+      <c r="I17" s="71"/>
     </row>
     <row r="18" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
@@ -1695,13 +1688,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E18" s="36" t="s">
+      <c r="E18" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="38"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="68"/>
     </row>
     <row r="19" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
@@ -1713,11 +1706,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E19" s="36"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="38"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="68"/>
     </row>
     <row r="20" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
@@ -1729,11 +1722,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E20" s="39"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="41"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="70"/>
+      <c r="H20" s="70"/>
+      <c r="I20" s="71"/>
     </row>
     <row r="21" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
@@ -1749,13 +1742,13 @@
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E21" s="39" t="s">
+      <c r="E21" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="41"/>
+      <c r="F21" s="70"/>
+      <c r="G21" s="70"/>
+      <c r="H21" s="70"/>
+      <c r="I21" s="71"/>
     </row>
     <row r="22" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
@@ -1767,11 +1760,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E22" s="39"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="41"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="71"/>
     </row>
     <row r="23" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
@@ -1783,11 +1776,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E23" s="39"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="41"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="70"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="70"/>
+      <c r="I23" s="71"/>
     </row>
     <row r="24" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
@@ -1799,11 +1792,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E24" s="39"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="41"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="70"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="70"/>
+      <c r="I24" s="71"/>
     </row>
     <row r="25" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
@@ -1815,11 +1808,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E25" s="36"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="38"/>
+      <c r="E25" s="66"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="67"/>
+      <c r="H25" s="67"/>
+      <c r="I25" s="68"/>
     </row>
     <row r="26" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
@@ -1831,11 +1824,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E26" s="36"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="38"/>
+      <c r="E26" s="66"/>
+      <c r="F26" s="67"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="67"/>
+      <c r="I26" s="68"/>
     </row>
     <row r="27" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
@@ -1851,13 +1844,13 @@
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E27" s="39" t="s">
+      <c r="E27" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="41"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="70"/>
+      <c r="H27" s="70"/>
+      <c r="I27" s="71"/>
     </row>
     <row r="28" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
@@ -1873,13 +1866,13 @@
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E28" s="39" t="s">
+      <c r="E28" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="F28" s="40"/>
-      <c r="G28" s="40"/>
-      <c r="H28" s="40"/>
-      <c r="I28" s="41"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="70"/>
+      <c r="H28" s="70"/>
+      <c r="I28" s="71"/>
     </row>
     <row r="29" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="29" t="s">
@@ -1895,13 +1888,13 @@
         <f t="shared" si="0"/>
         <v>4.1666666666666741E-2</v>
       </c>
-      <c r="E29" s="39" t="s">
+      <c r="E29" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="41"/>
+      <c r="F29" s="70"/>
+      <c r="G29" s="70"/>
+      <c r="H29" s="70"/>
+      <c r="I29" s="71"/>
     </row>
     <row r="30" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="29" t="s">
@@ -1913,11 +1906,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E30" s="39"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="41"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="70"/>
+      <c r="G30" s="70"/>
+      <c r="H30" s="70"/>
+      <c r="I30" s="71"/>
     </row>
     <row r="31" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
@@ -1933,13 +1926,13 @@
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="E31" s="39" t="s">
+      <c r="E31" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="41"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="70"/>
+      <c r="I31" s="71"/>
     </row>
     <row r="32" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
@@ -1951,11 +1944,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E32" s="36"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="37"/>
-      <c r="H32" s="37"/>
-      <c r="I32" s="38"/>
+      <c r="E32" s="66"/>
+      <c r="F32" s="67"/>
+      <c r="G32" s="67"/>
+      <c r="H32" s="67"/>
+      <c r="I32" s="68"/>
     </row>
     <row r="33" spans="1:13" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
@@ -1967,11 +1960,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E33" s="36"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="38"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="67"/>
+      <c r="G33" s="67"/>
+      <c r="H33" s="67"/>
+      <c r="I33" s="68"/>
     </row>
     <row r="34" spans="1:13" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="s">
@@ -1983,11 +1976,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E34" s="39"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="41"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="70"/>
+      <c r="H34" s="70"/>
+      <c r="I34" s="71"/>
     </row>
     <row r="35" spans="1:13" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
@@ -1999,11 +1992,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E35" s="39"/>
-      <c r="F35" s="40"/>
-      <c r="G35" s="40"/>
-      <c r="H35" s="40"/>
-      <c r="I35" s="41"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="70"/>
+      <c r="H35" s="70"/>
+      <c r="I35" s="71"/>
     </row>
     <row r="36" spans="1:13" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="29" t="s">
@@ -2019,13 +2012,13 @@
         <f t="shared" si="0"/>
         <v>2.083333333333337E-2</v>
       </c>
-      <c r="E36" s="39" t="s">
+      <c r="E36" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="F36" s="40"/>
-      <c r="G36" s="40"/>
-      <c r="H36" s="40"/>
-      <c r="I36" s="41"/>
+      <c r="F36" s="70"/>
+      <c r="G36" s="70"/>
+      <c r="H36" s="70"/>
+      <c r="I36" s="71"/>
     </row>
     <row r="37" spans="1:13" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="29" t="s">
@@ -2037,11 +2030,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="40"/>
-      <c r="G37" s="40"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="41"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="70"/>
+      <c r="G37" s="70"/>
+      <c r="H37" s="70"/>
+      <c r="I37" s="71"/>
     </row>
     <row r="38" spans="1:13" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="29" t="s">
@@ -2053,11 +2046,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E38" s="39"/>
-      <c r="F38" s="40"/>
-      <c r="G38" s="40"/>
-      <c r="H38" s="40"/>
-      <c r="I38" s="41"/>
+      <c r="E38" s="69"/>
+      <c r="F38" s="70"/>
+      <c r="G38" s="70"/>
+      <c r="H38" s="70"/>
+      <c r="I38" s="71"/>
     </row>
     <row r="39" spans="1:13" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
@@ -2069,11 +2062,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E39" s="36"/>
-      <c r="F39" s="37"/>
-      <c r="G39" s="37"/>
-      <c r="H39" s="37"/>
-      <c r="I39" s="38"/>
+      <c r="E39" s="66"/>
+      <c r="F39" s="67"/>
+      <c r="G39" s="67"/>
+      <c r="H39" s="67"/>
+      <c r="I39" s="68"/>
     </row>
     <row r="40" spans="1:13" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
@@ -2089,13 +2082,13 @@
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E40" s="36" t="s">
+      <c r="E40" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="F40" s="37"/>
-      <c r="G40" s="37"/>
-      <c r="H40" s="37"/>
-      <c r="I40" s="38"/>
+      <c r="F40" s="67"/>
+      <c r="G40" s="67"/>
+      <c r="H40" s="67"/>
+      <c r="I40" s="68"/>
     </row>
     <row r="41" spans="1:13" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="29" t="s">
@@ -2107,11 +2100,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E41" s="39"/>
-      <c r="F41" s="40"/>
-      <c r="G41" s="40"/>
-      <c r="H41" s="40"/>
-      <c r="I41" s="41"/>
+      <c r="E41" s="69"/>
+      <c r="F41" s="70"/>
+      <c r="G41" s="70"/>
+      <c r="H41" s="70"/>
+      <c r="I41" s="71"/>
     </row>
     <row r="42" spans="1:13" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="29" t="s">
@@ -2123,11 +2116,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E42" s="39"/>
-      <c r="F42" s="40"/>
-      <c r="G42" s="40"/>
-      <c r="H42" s="40"/>
-      <c r="I42" s="41"/>
+      <c r="E42" s="69"/>
+      <c r="F42" s="70"/>
+      <c r="G42" s="70"/>
+      <c r="H42" s="70"/>
+      <c r="I42" s="71"/>
     </row>
     <row r="43" spans="1:13" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="29" t="s">
@@ -2139,11 +2132,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E43" s="39"/>
-      <c r="F43" s="40"/>
-      <c r="G43" s="40"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="41"/>
+      <c r="E43" s="69"/>
+      <c r="F43" s="70"/>
+      <c r="G43" s="70"/>
+      <c r="H43" s="70"/>
+      <c r="I43" s="71"/>
     </row>
     <row r="44" spans="1:13" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="29" t="s">
@@ -2155,11 +2148,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E44" s="39"/>
-      <c r="F44" s="40"/>
-      <c r="G44" s="40"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="41"/>
+      <c r="E44" s="69"/>
+      <c r="F44" s="70"/>
+      <c r="G44" s="70"/>
+      <c r="H44" s="70"/>
+      <c r="I44" s="71"/>
     </row>
     <row r="45" spans="1:13" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="29" t="s">
@@ -2175,13 +2168,13 @@
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E45" s="39" t="s">
+      <c r="E45" s="69" t="s">
         <v>54</v>
       </c>
-      <c r="F45" s="40"/>
-      <c r="G45" s="40"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="41"/>
+      <c r="F45" s="70"/>
+      <c r="G45" s="70"/>
+      <c r="H45" s="70"/>
+      <c r="I45" s="71"/>
     </row>
     <row r="46" spans="1:13" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="25" t="s">
@@ -2193,25 +2186,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E46" s="36"/>
-      <c r="F46" s="37"/>
-      <c r="G46" s="37"/>
-      <c r="H46" s="37"/>
-      <c r="I46" s="38"/>
+      <c r="E46" s="66"/>
+      <c r="F46" s="67"/>
+      <c r="G46" s="67"/>
+      <c r="H46" s="67"/>
+      <c r="I46" s="68"/>
     </row>
     <row r="47" spans="1:13" s="24" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A47" s="42"/>
-      <c r="B47" s="43"/>
-      <c r="C47" s="43"/>
+      <c r="A47" s="73"/>
+      <c r="B47" s="74"/>
+      <c r="C47" s="74"/>
       <c r="D47" s="23">
         <f>SUM(D16:D46)</f>
         <v>0.54166666666666696</v>
       </c>
-      <c r="E47" s="44"/>
-      <c r="F47" s="44"/>
-      <c r="G47" s="44"/>
-      <c r="H47" s="44"/>
-      <c r="I47" s="45"/>
+      <c r="E47" s="75"/>
+      <c r="F47" s="75"/>
+      <c r="G47" s="75"/>
+      <c r="H47" s="75"/>
+      <c r="I47" s="76"/>
     </row>
     <row r="48" spans="1:13" ht="7.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="18"/>
@@ -2242,35 +2235,19 @@
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:I15"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="E19:I19"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E39:I39"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="E41:I41"/>
+    <mergeCell ref="E36:I36"/>
+    <mergeCell ref="E37:I37"/>
+    <mergeCell ref="E38:I38"/>
+    <mergeCell ref="E45:I45"/>
+    <mergeCell ref="E46:I46"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="E47:I47"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="E44:I44"/>
     <mergeCell ref="E35:I35"/>
     <mergeCell ref="E30:I30"/>
     <mergeCell ref="E31:I31"/>
@@ -2280,19 +2257,35 @@
     <mergeCell ref="E29:I29"/>
     <mergeCell ref="E33:I33"/>
     <mergeCell ref="E34:I34"/>
-    <mergeCell ref="E45:I45"/>
-    <mergeCell ref="E46:I46"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="E47:I47"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="E44:I44"/>
-    <mergeCell ref="E39:I39"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="E41:I41"/>
-    <mergeCell ref="E36:I36"/>
-    <mergeCell ref="E37:I37"/>
-    <mergeCell ref="E38:I38"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="E19:I19"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:I15"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A8:I8"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.44" right="0.03" top="0.02" bottom="0.03" header="0.19685039370078741" footer="0.19685039370078741"/>
@@ -2308,7 +2301,7 @@
   </sheetPr>
   <dimension ref="A1:AR47"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A23" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="E42" sqref="E42:I42"/>
     </sheetView>
   </sheetViews>
@@ -2328,18 +2321,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" s="6" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="str">
+      <c r="A1" s="36" t="str">
         <f>October!A1</f>
         <v>Monthly timesheet for MSc Geoinformatics ip:sdi - 23W856162</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -2377,126 +2370,126 @@
       <c r="AR1" s="1"/>
     </row>
     <row r="2" spans="1:44" s="1" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="73"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
     </row>
     <row r="3" spans="1:44" s="7" customFormat="1" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
       <c r="I3" s="14"/>
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
     </row>
     <row r="4" spans="1:44" s="1" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="75"/>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:44" s="1" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="64" t="str">
+      <c r="A5" s="42" t="str">
         <f>October!A5</f>
         <v>Firstname Lastname</v>
       </c>
-      <c r="B5" s="65"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="66" t="str">
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="44" t="str">
         <f>October!D5</f>
         <v>Stamatina Tounta</v>
       </c>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="68"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="46"/>
       <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:44" s="1" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="69"/>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="69"/>
-      <c r="H6" s="69"/>
-      <c r="I6" s="69"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
     </row>
     <row r="7" spans="1:44" s="1" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="70" t="str">
+      <c r="A7" s="48" t="str">
         <f>October!A7</f>
         <v>Project Acronym</v>
       </c>
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="71" t="str">
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="49" t="str">
         <f>October!D7</f>
         <v>SudMig</v>
       </c>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
       <c r="I7" s="15"/>
     </row>
     <row r="8" spans="1:44" s="1" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="76"/>
-      <c r="B8" s="76"/>
-      <c r="C8" s="76"/>
-      <c r="D8" s="76"/>
-      <c r="E8" s="76"/>
-      <c r="F8" s="76"/>
-      <c r="G8" s="76"/>
-      <c r="H8" s="76"/>
-      <c r="I8" s="76"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
     </row>
     <row r="9" spans="1:44" s="1" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="70" t="str">
+      <c r="A9" s="48" t="str">
         <f>October!A9</f>
         <v>Project Title</v>
       </c>
-      <c r="B9" s="70"/>
-      <c r="C9" s="70"/>
-      <c r="D9" s="66" t="str">
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="44" t="str">
         <f>October!D9</f>
         <v>Sudan: monitoring migrant movements related to the 2023 conflict</v>
       </c>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="68"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="46"/>
       <c r="I9" s="15"/>
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:44" s="1" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="63"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="63"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
     </row>
     <row r="11" spans="1:44" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
@@ -2526,51 +2519,51 @@
       <c r="I12" s="16"/>
     </row>
     <row r="13" spans="1:44" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="52"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="55"/>
     </row>
     <row r="14" spans="1:44" s="2" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="48"/>
-      <c r="B14" s="53" t="s">
+      <c r="A14" s="51"/>
+      <c r="B14" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="54"/>
-      <c r="D14" s="55" t="s">
+      <c r="C14" s="57"/>
+      <c r="D14" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="57" t="s">
+      <c r="E14" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="58"/>
-      <c r="G14" s="58"/>
-      <c r="H14" s="58"/>
-      <c r="I14" s="59"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="62"/>
     </row>
     <row r="15" spans="1:44" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="49"/>
+      <c r="A15" s="52"/>
       <c r="B15" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="56"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
-      <c r="H15" s="61"/>
-      <c r="I15" s="62"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="64"/>
+      <c r="I15" s="65"/>
     </row>
     <row r="16" spans="1:44" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
@@ -2582,11 +2575,11 @@
         <f>C16-B16</f>
         <v>0</v>
       </c>
-      <c r="E16" s="36"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="38"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="68"/>
     </row>
     <row r="17" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
@@ -2598,11 +2591,11 @@
         <f t="shared" ref="D17:D45" si="0">C17-B17</f>
         <v>0</v>
       </c>
-      <c r="E17" s="39"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="41"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="70"/>
+      <c r="I17" s="71"/>
     </row>
     <row r="18" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
@@ -2618,13 +2611,13 @@
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E18" s="39" t="s">
+      <c r="E18" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="41"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="70"/>
+      <c r="H18" s="70"/>
+      <c r="I18" s="71"/>
     </row>
     <row r="19" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
@@ -2636,11 +2629,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E19" s="39"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="41"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="70"/>
+      <c r="H19" s="70"/>
+      <c r="I19" s="71"/>
     </row>
     <row r="20" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
@@ -2652,11 +2645,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E20" s="39"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="41"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="70"/>
+      <c r="H20" s="70"/>
+      <c r="I20" s="71"/>
     </row>
     <row r="21" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
@@ -2672,13 +2665,13 @@
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E21" s="39" t="s">
+      <c r="E21" s="69" t="s">
         <v>57</v>
       </c>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="41"/>
+      <c r="F21" s="70"/>
+      <c r="G21" s="70"/>
+      <c r="H21" s="70"/>
+      <c r="I21" s="71"/>
     </row>
     <row r="22" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
@@ -2690,11 +2683,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E22" s="36"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="38"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="68"/>
     </row>
     <row r="23" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
@@ -2706,11 +2699,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E23" s="36"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="38"/>
+      <c r="E23" s="66"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="67"/>
+      <c r="I23" s="68"/>
     </row>
     <row r="24" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
@@ -2726,13 +2719,13 @@
         <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
-      <c r="E24" s="39" t="s">
+      <c r="E24" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="41"/>
+      <c r="F24" s="70"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="70"/>
+      <c r="I24" s="71"/>
     </row>
     <row r="25" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
@@ -2744,11 +2737,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E25" s="39"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="41"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="70"/>
+      <c r="G25" s="70"/>
+      <c r="H25" s="70"/>
+      <c r="I25" s="71"/>
     </row>
     <row r="26" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
@@ -2760,11 +2753,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E26" s="39"/>
-      <c r="F26" s="40"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="41"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="70"/>
+      <c r="G26" s="70"/>
+      <c r="H26" s="70"/>
+      <c r="I26" s="71"/>
     </row>
     <row r="27" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
@@ -2776,11 +2769,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E27" s="39"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="41"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="70"/>
+      <c r="H27" s="70"/>
+      <c r="I27" s="71"/>
     </row>
     <row r="28" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
@@ -2796,13 +2789,13 @@
         <f t="shared" si="0"/>
         <v>4.1666666666666741E-2</v>
       </c>
-      <c r="E28" s="39" t="s">
+      <c r="E28" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="F28" s="40"/>
-      <c r="G28" s="40"/>
-      <c r="H28" s="40"/>
-      <c r="I28" s="41"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="70"/>
+      <c r="H28" s="70"/>
+      <c r="I28" s="71"/>
     </row>
     <row r="29" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
@@ -2814,11 +2807,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E29" s="36"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="38"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="67"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="67"/>
+      <c r="I29" s="68"/>
     </row>
     <row r="30" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
@@ -2834,13 +2827,13 @@
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E30" s="36" t="s">
+      <c r="E30" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="38"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="67"/>
+      <c r="H30" s="67"/>
+      <c r="I30" s="68"/>
     </row>
     <row r="31" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
@@ -2856,13 +2849,13 @@
         <f t="shared" si="0"/>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="E31" s="39" t="s">
+      <c r="E31" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="41"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="70"/>
+      <c r="I31" s="71"/>
     </row>
     <row r="32" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="29" t="s">
@@ -2874,11 +2867,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E32" s="39"/>
-      <c r="F32" s="40"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="40"/>
-      <c r="I32" s="41"/>
+      <c r="E32" s="69"/>
+      <c r="F32" s="70"/>
+      <c r="G32" s="70"/>
+      <c r="H32" s="70"/>
+      <c r="I32" s="71"/>
     </row>
     <row r="33" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="29" t="s">
@@ -2890,11 +2883,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E33" s="39"/>
-      <c r="F33" s="40"/>
-      <c r="G33" s="40"/>
-      <c r="H33" s="40"/>
-      <c r="I33" s="41"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="70"/>
+      <c r="G33" s="70"/>
+      <c r="H33" s="70"/>
+      <c r="I33" s="71"/>
     </row>
     <row r="34" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="s">
@@ -2906,11 +2899,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E34" s="39"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="41"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="70"/>
+      <c r="H34" s="70"/>
+      <c r="I34" s="71"/>
     </row>
     <row r="35" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
@@ -2926,13 +2919,13 @@
         <f t="shared" si="0"/>
         <v>8.3333333333333259E-2</v>
       </c>
-      <c r="E35" s="39" t="s">
+      <c r="E35" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="F35" s="40"/>
-      <c r="G35" s="40"/>
-      <c r="H35" s="40"/>
-      <c r="I35" s="41"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="70"/>
+      <c r="H35" s="70"/>
+      <c r="I35" s="71"/>
     </row>
     <row r="36" spans="1:12" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
@@ -2944,11 +2937,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="37"/>
-      <c r="G36" s="37"/>
-      <c r="H36" s="37"/>
-      <c r="I36" s="38"/>
+      <c r="E36" s="66"/>
+      <c r="F36" s="67"/>
+      <c r="G36" s="67"/>
+      <c r="H36" s="67"/>
+      <c r="I36" s="68"/>
     </row>
     <row r="37" spans="1:12" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
@@ -2960,11 +2953,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="37"/>
-      <c r="H37" s="37"/>
-      <c r="I37" s="38"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="67"/>
+      <c r="G37" s="67"/>
+      <c r="H37" s="67"/>
+      <c r="I37" s="68"/>
     </row>
     <row r="38" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="29" t="s">
@@ -2980,13 +2973,13 @@
         <f t="shared" si="0"/>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="E38" s="39" t="s">
+      <c r="E38" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="F38" s="40"/>
-      <c r="G38" s="40"/>
-      <c r="H38" s="40"/>
-      <c r="I38" s="41"/>
+      <c r="F38" s="70"/>
+      <c r="G38" s="70"/>
+      <c r="H38" s="70"/>
+      <c r="I38" s="71"/>
     </row>
     <row r="39" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="29" t="s">
@@ -2998,11 +2991,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E39" s="39"/>
-      <c r="F39" s="40"/>
-      <c r="G39" s="40"/>
-      <c r="H39" s="40"/>
-      <c r="I39" s="41"/>
+      <c r="E39" s="69"/>
+      <c r="F39" s="70"/>
+      <c r="G39" s="70"/>
+      <c r="H39" s="70"/>
+      <c r="I39" s="71"/>
     </row>
     <row r="40" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="29" t="s">
@@ -3018,13 +3011,13 @@
         <f t="shared" si="0"/>
         <v>4.1666666666666741E-2</v>
       </c>
-      <c r="E40" s="39" t="s">
+      <c r="E40" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="F40" s="40"/>
-      <c r="G40" s="40"/>
-      <c r="H40" s="40"/>
-      <c r="I40" s="41"/>
+      <c r="F40" s="70"/>
+      <c r="G40" s="70"/>
+      <c r="H40" s="70"/>
+      <c r="I40" s="71"/>
     </row>
     <row r="41" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="29" t="s">
@@ -3036,11 +3029,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E41" s="39"/>
-      <c r="F41" s="40"/>
-      <c r="G41" s="40"/>
-      <c r="H41" s="40"/>
-      <c r="I41" s="41"/>
+      <c r="E41" s="69"/>
+      <c r="F41" s="70"/>
+      <c r="G41" s="70"/>
+      <c r="H41" s="70"/>
+      <c r="I41" s="71"/>
     </row>
     <row r="42" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="29" t="s">
@@ -3056,13 +3049,13 @@
         <f t="shared" si="0"/>
         <v>2.0833333333333259E-2</v>
       </c>
-      <c r="E42" s="39" t="s">
+      <c r="E42" s="69" t="s">
         <v>64</v>
       </c>
-      <c r="F42" s="40"/>
-      <c r="G42" s="40"/>
-      <c r="H42" s="40"/>
-      <c r="I42" s="41"/>
+      <c r="F42" s="70"/>
+      <c r="G42" s="70"/>
+      <c r="H42" s="70"/>
+      <c r="I42" s="71"/>
     </row>
     <row r="43" spans="1:12" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
@@ -3074,11 +3067,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E43" s="36"/>
-      <c r="F43" s="37"/>
-      <c r="G43" s="37"/>
-      <c r="H43" s="37"/>
-      <c r="I43" s="38"/>
+      <c r="E43" s="66"/>
+      <c r="F43" s="67"/>
+      <c r="G43" s="67"/>
+      <c r="H43" s="67"/>
+      <c r="I43" s="68"/>
     </row>
     <row r="44" spans="1:12" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="25" t="s">
@@ -3094,13 +3087,13 @@
         <f t="shared" si="0"/>
         <v>8.3333333333333259E-2</v>
       </c>
-      <c r="E44" s="36" t="s">
+      <c r="E44" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="F44" s="37"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="37"/>
-      <c r="I44" s="38"/>
+      <c r="F44" s="67"/>
+      <c r="G44" s="67"/>
+      <c r="H44" s="67"/>
+      <c r="I44" s="68"/>
     </row>
     <row r="45" spans="1:12" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="29" t="s">
@@ -3116,27 +3109,27 @@
         <f t="shared" si="0"/>
         <v>4.1666666666666685E-2</v>
       </c>
-      <c r="E45" s="39" t="s">
+      <c r="E45" s="69" t="s">
         <v>66</v>
       </c>
-      <c r="F45" s="40"/>
-      <c r="G45" s="40"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="41"/>
+      <c r="F45" s="70"/>
+      <c r="G45" s="70"/>
+      <c r="H45" s="70"/>
+      <c r="I45" s="71"/>
     </row>
     <row r="46" spans="1:12" s="24" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A46" s="42"/>
-      <c r="B46" s="43"/>
-      <c r="C46" s="43"/>
+      <c r="A46" s="73"/>
+      <c r="B46" s="74"/>
+      <c r="C46" s="74"/>
       <c r="D46" s="23">
         <f>SUM(D16:D45)</f>
         <v>0.70833333333333326</v>
       </c>
-      <c r="E46" s="44"/>
-      <c r="F46" s="44"/>
-      <c r="G46" s="44"/>
-      <c r="H46" s="44"/>
-      <c r="I46" s="45"/>
+      <c r="E46" s="75"/>
+      <c r="F46" s="75"/>
+      <c r="G46" s="75"/>
+      <c r="H46" s="75"/>
+      <c r="I46" s="76"/>
     </row>
     <row r="47" spans="1:12" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="18"/>
@@ -3154,6 +3147,40 @@
     </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="E46:I46"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="E44:I44"/>
+    <mergeCell ref="E45:I45"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="E41:I41"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="E37:I37"/>
+    <mergeCell ref="E38:I38"/>
+    <mergeCell ref="E39:I39"/>
+    <mergeCell ref="E34:I34"/>
+    <mergeCell ref="E35:I35"/>
+    <mergeCell ref="E36:I36"/>
+    <mergeCell ref="E31:I31"/>
+    <mergeCell ref="E32:I32"/>
+    <mergeCell ref="E33:I33"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="E30:I30"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="E20:I20"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A3:H3"/>
@@ -3170,40 +3197,6 @@
     <mergeCell ref="E14:I15"/>
     <mergeCell ref="E16:I16"/>
     <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="E22:I22"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E24:I24"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="E28:I28"/>
-    <mergeCell ref="E29:I29"/>
-    <mergeCell ref="E30:I30"/>
-    <mergeCell ref="E25:I25"/>
-    <mergeCell ref="E26:I26"/>
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E35:I35"/>
-    <mergeCell ref="E36:I36"/>
-    <mergeCell ref="E31:I31"/>
-    <mergeCell ref="E32:I32"/>
-    <mergeCell ref="E33:I33"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="E46:I46"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="E44:I44"/>
-    <mergeCell ref="E45:I45"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="E41:I41"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="E37:I37"/>
-    <mergeCell ref="E38:I38"/>
-    <mergeCell ref="E39:I39"/>
-    <mergeCell ref="E34:I34"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.44" right="0.03" top="0.02" bottom="0.03" header="0.19685039370078741" footer="0.19685039370078741"/>
@@ -3219,7 +3212,7 @@
   </sheetPr>
   <dimension ref="A1:AM49"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A27" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="E47" sqref="E47:I47"/>
     </sheetView>
   </sheetViews>
@@ -3238,18 +3231,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" s="6" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="str">
+      <c r="A1" s="36" t="str">
         <f>October!A1</f>
         <v>Monthly timesheet for MSc Geoinformatics ip:sdi - 23W856162</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -3282,126 +3275,126 @@
       <c r="AM1" s="1"/>
     </row>
     <row r="2" spans="1:39" s="1" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="73"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
     </row>
     <row r="3" spans="1:39" s="7" customFormat="1" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
       <c r="I3" s="14"/>
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
     </row>
     <row r="4" spans="1:39" s="1" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="75"/>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:39" s="1" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="64" t="str">
+      <c r="A5" s="42" t="str">
         <f>October!A5</f>
         <v>Firstname Lastname</v>
       </c>
-      <c r="B5" s="65"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="66" t="str">
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="44" t="str">
         <f>October!D5</f>
         <v>Stamatina Tounta</v>
       </c>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="68"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="46"/>
       <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:39" s="1" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="69"/>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="69"/>
-      <c r="H6" s="69"/>
-      <c r="I6" s="69"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
     </row>
     <row r="7" spans="1:39" s="1" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="70" t="str">
+      <c r="A7" s="48" t="str">
         <f>October!A7</f>
         <v>Project Acronym</v>
       </c>
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="71" t="str">
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="49" t="str">
         <f>October!D7</f>
         <v>SudMig</v>
       </c>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
       <c r="I7" s="15"/>
     </row>
     <row r="8" spans="1:39" s="1" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="76"/>
-      <c r="B8" s="76"/>
-      <c r="C8" s="76"/>
-      <c r="D8" s="76"/>
-      <c r="E8" s="76"/>
-      <c r="F8" s="76"/>
-      <c r="G8" s="76"/>
-      <c r="H8" s="76"/>
-      <c r="I8" s="76"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
     </row>
     <row r="9" spans="1:39" s="1" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="70" t="str">
+      <c r="A9" s="48" t="str">
         <f>October!A9</f>
         <v>Project Title</v>
       </c>
-      <c r="B9" s="70"/>
-      <c r="C9" s="70"/>
-      <c r="D9" s="66" t="str">
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="44" t="str">
         <f>October!D9</f>
         <v>Sudan: monitoring migrant movements related to the 2023 conflict</v>
       </c>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="68"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="46"/>
       <c r="I9" s="15"/>
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:39" s="1" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="63"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="63"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
     </row>
     <row r="11" spans="1:39" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
@@ -3431,51 +3424,51 @@
       <c r="I12" s="16"/>
     </row>
     <row r="13" spans="1:39" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="52"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="55"/>
     </row>
     <row r="14" spans="1:39" s="2" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="48"/>
-      <c r="B14" s="53" t="s">
+      <c r="A14" s="51"/>
+      <c r="B14" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="54"/>
-      <c r="D14" s="55" t="s">
+      <c r="C14" s="57"/>
+      <c r="D14" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="57" t="s">
+      <c r="E14" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="58"/>
-      <c r="G14" s="58"/>
-      <c r="H14" s="58"/>
-      <c r="I14" s="59"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="62"/>
     </row>
     <row r="15" spans="1:39" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="49"/>
+      <c r="A15" s="52"/>
       <c r="B15" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="56"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
-      <c r="H15" s="61"/>
-      <c r="I15" s="62"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="64"/>
+      <c r="I15" s="65"/>
     </row>
     <row r="16" spans="1:39" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="77" t="s">
@@ -3491,13 +3484,13 @@
         <f t="shared" ref="D16:D47" si="0">C16-B16</f>
         <v>4.1666666666666685E-2</v>
       </c>
-      <c r="E16" s="39" t="s">
+      <c r="E16" s="69" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="41"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="70"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="71"/>
     </row>
     <row r="17" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="78"/>
@@ -3511,12 +3504,12 @@
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E17" s="39" t="s">
+      <c r="E17" s="69" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="70"/>
       <c r="I17" s="35"/>
     </row>
     <row r="18" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
@@ -3529,11 +3522,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E18" s="39"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="41"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="70"/>
+      <c r="H18" s="70"/>
+      <c r="I18" s="71"/>
     </row>
     <row r="19" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
@@ -3549,13 +3542,13 @@
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E19" s="39" t="s">
+      <c r="E19" s="69" t="s">
         <v>69</v>
       </c>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="41"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="70"/>
+      <c r="H19" s="70"/>
+      <c r="I19" s="71"/>
     </row>
     <row r="20" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
@@ -3567,11 +3560,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E20" s="39"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="41"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="70"/>
+      <c r="H20" s="70"/>
+      <c r="I20" s="71"/>
     </row>
     <row r="21" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
@@ -3583,11 +3576,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E21" s="36"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="38"/>
+      <c r="E21" s="66"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="68"/>
     </row>
     <row r="22" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
@@ -3599,11 +3592,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E22" s="36"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="38"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="68"/>
     </row>
     <row r="23" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
@@ -3615,11 +3608,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E23" s="39"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="41"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="70"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="70"/>
+      <c r="I23" s="71"/>
     </row>
     <row r="24" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
@@ -3631,11 +3624,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E24" s="39"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="41"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="70"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="70"/>
+      <c r="I24" s="71"/>
     </row>
     <row r="25" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
@@ -3647,11 +3640,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E25" s="39"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="41"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="70"/>
+      <c r="G25" s="70"/>
+      <c r="H25" s="70"/>
+      <c r="I25" s="71"/>
     </row>
     <row r="26" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
@@ -3663,11 +3656,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E26" s="39"/>
-      <c r="F26" s="40"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="41"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="70"/>
+      <c r="G26" s="70"/>
+      <c r="H26" s="70"/>
+      <c r="I26" s="71"/>
     </row>
     <row r="27" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
@@ -3679,11 +3672,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E27" s="39"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="41"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="70"/>
+      <c r="H27" s="70"/>
+      <c r="I27" s="71"/>
     </row>
     <row r="28" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
@@ -3695,11 +3688,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E28" s="36"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="38"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="67"/>
+      <c r="I28" s="68"/>
     </row>
     <row r="29" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
@@ -3711,11 +3704,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E29" s="36"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="38"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="67"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="67"/>
+      <c r="I29" s="68"/>
     </row>
     <row r="30" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="29" t="s">
@@ -3727,11 +3720,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E30" s="39"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="41"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="70"/>
+      <c r="G30" s="70"/>
+      <c r="H30" s="70"/>
+      <c r="I30" s="71"/>
     </row>
     <row r="31" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
@@ -3743,11 +3736,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E31" s="39"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="41"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="70"/>
+      <c r="I31" s="71"/>
     </row>
     <row r="32" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="29" t="s">
@@ -3759,11 +3752,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E32" s="39"/>
-      <c r="F32" s="40"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="40"/>
-      <c r="I32" s="41"/>
+      <c r="E32" s="69"/>
+      <c r="F32" s="70"/>
+      <c r="G32" s="70"/>
+      <c r="H32" s="70"/>
+      <c r="I32" s="71"/>
     </row>
     <row r="33" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="29" t="s">
@@ -3779,13 +3772,13 @@
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E33" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="F33" s="40"/>
-      <c r="G33" s="40"/>
-      <c r="H33" s="40"/>
-      <c r="I33" s="41"/>
+      <c r="E33" s="69" t="s">
+        <v>70</v>
+      </c>
+      <c r="F33" s="70"/>
+      <c r="G33" s="70"/>
+      <c r="H33" s="70"/>
+      <c r="I33" s="71"/>
     </row>
     <row r="34" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="29" t="s">
@@ -3797,11 +3790,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E34" s="39"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="41"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="70"/>
+      <c r="G34" s="70"/>
+      <c r="H34" s="70"/>
+      <c r="I34" s="71"/>
     </row>
     <row r="35" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
@@ -3813,11 +3806,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E35" s="36"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="37"/>
-      <c r="H35" s="37"/>
-      <c r="I35" s="38"/>
+      <c r="E35" s="66"/>
+      <c r="F35" s="67"/>
+      <c r="G35" s="67"/>
+      <c r="H35" s="67"/>
+      <c r="I35" s="68"/>
     </row>
     <row r="36" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
@@ -3833,13 +3826,13 @@
         <f t="shared" si="0"/>
         <v>0.16666666666666663</v>
       </c>
-      <c r="E36" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="F36" s="37"/>
-      <c r="G36" s="37"/>
-      <c r="H36" s="37"/>
-      <c r="I36" s="38"/>
+      <c r="E36" s="66" t="s">
+        <v>71</v>
+      </c>
+      <c r="F36" s="67"/>
+      <c r="G36" s="67"/>
+      <c r="H36" s="67"/>
+      <c r="I36" s="68"/>
     </row>
     <row r="37" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="29" t="s">
@@ -3855,13 +3848,13 @@
         <f t="shared" si="0"/>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E37" s="39" t="s">
-        <v>71</v>
-      </c>
-      <c r="F37" s="40"/>
-      <c r="G37" s="40"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="41"/>
+      <c r="E37" s="69" t="s">
+        <v>72</v>
+      </c>
+      <c r="F37" s="70"/>
+      <c r="G37" s="70"/>
+      <c r="H37" s="70"/>
+      <c r="I37" s="71"/>
     </row>
     <row r="38" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="29" t="s">
@@ -3877,13 +3870,13 @@
         <f t="shared" si="0"/>
         <v>8.3333333333333259E-2</v>
       </c>
-      <c r="E38" s="39" t="s">
+      <c r="E38" s="69" t="s">
         <v>73</v>
       </c>
-      <c r="F38" s="40"/>
-      <c r="G38" s="40"/>
-      <c r="H38" s="40"/>
-      <c r="I38" s="41"/>
+      <c r="F38" s="70"/>
+      <c r="G38" s="70"/>
+      <c r="H38" s="70"/>
+      <c r="I38" s="71"/>
     </row>
     <row r="39" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="29" t="s">
@@ -3895,11 +3888,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E39" s="39"/>
-      <c r="F39" s="40"/>
-      <c r="G39" s="40"/>
-      <c r="H39" s="40"/>
-      <c r="I39" s="41"/>
+      <c r="E39" s="69"/>
+      <c r="F39" s="70"/>
+      <c r="G39" s="70"/>
+      <c r="H39" s="70"/>
+      <c r="I39" s="71"/>
     </row>
     <row r="40" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="29" t="s">
@@ -3911,11 +3904,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E40" s="39"/>
-      <c r="F40" s="40"/>
-      <c r="G40" s="40"/>
-      <c r="H40" s="40"/>
-      <c r="I40" s="41"/>
+      <c r="E40" s="69"/>
+      <c r="F40" s="70"/>
+      <c r="G40" s="70"/>
+      <c r="H40" s="70"/>
+      <c r="I40" s="71"/>
     </row>
     <row r="41" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="29" t="s">
@@ -3927,11 +3920,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E41" s="39"/>
-      <c r="F41" s="40"/>
-      <c r="G41" s="40"/>
-      <c r="H41" s="40"/>
-      <c r="I41" s="41"/>
+      <c r="E41" s="69"/>
+      <c r="F41" s="70"/>
+      <c r="G41" s="70"/>
+      <c r="H41" s="70"/>
+      <c r="I41" s="71"/>
     </row>
     <row r="42" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="25" t="s">
@@ -3943,11 +3936,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E42" s="36"/>
-      <c r="F42" s="37"/>
-      <c r="G42" s="37"/>
-      <c r="H42" s="37"/>
-      <c r="I42" s="38"/>
+      <c r="E42" s="66"/>
+      <c r="F42" s="67"/>
+      <c r="G42" s="67"/>
+      <c r="H42" s="67"/>
+      <c r="I42" s="68"/>
     </row>
     <row r="43" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
@@ -3959,11 +3952,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E43" s="36"/>
-      <c r="F43" s="37"/>
-      <c r="G43" s="37"/>
-      <c r="H43" s="37"/>
-      <c r="I43" s="38"/>
+      <c r="E43" s="66"/>
+      <c r="F43" s="67"/>
+      <c r="G43" s="67"/>
+      <c r="H43" s="67"/>
+      <c r="I43" s="68"/>
     </row>
     <row r="44" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="29" t="s">
@@ -3975,11 +3968,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E44" s="39"/>
-      <c r="F44" s="40"/>
-      <c r="G44" s="40"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="41"/>
+      <c r="E44" s="69"/>
+      <c r="F44" s="70"/>
+      <c r="G44" s="70"/>
+      <c r="H44" s="70"/>
+      <c r="I44" s="71"/>
     </row>
     <row r="45" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="29" t="s">
@@ -3995,13 +3988,13 @@
         <f t="shared" si="0"/>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="E45" s="39" t="s">
+      <c r="E45" s="69" t="s">
         <v>74</v>
       </c>
-      <c r="F45" s="40"/>
-      <c r="G45" s="40"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="41"/>
+      <c r="F45" s="70"/>
+      <c r="G45" s="70"/>
+      <c r="H45" s="70"/>
+      <c r="I45" s="71"/>
     </row>
     <row r="46" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="29" t="s">
@@ -4017,13 +4010,13 @@
         <f t="shared" si="0"/>
         <v>8.3333333333333315E-2</v>
       </c>
-      <c r="E46" s="39" t="s">
+      <c r="E46" s="69" t="s">
         <v>75</v>
       </c>
-      <c r="F46" s="40"/>
-      <c r="G46" s="40"/>
-      <c r="H46" s="40"/>
-      <c r="I46" s="41"/>
+      <c r="F46" s="70"/>
+      <c r="G46" s="70"/>
+      <c r="H46" s="70"/>
+      <c r="I46" s="71"/>
     </row>
     <row r="47" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="29" t="s">
@@ -4035,25 +4028,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E47" s="39"/>
-      <c r="F47" s="40"/>
-      <c r="G47" s="40"/>
-      <c r="H47" s="40"/>
-      <c r="I47" s="41"/>
+      <c r="E47" s="69"/>
+      <c r="F47" s="70"/>
+      <c r="G47" s="70"/>
+      <c r="H47" s="70"/>
+      <c r="I47" s="71"/>
     </row>
     <row r="48" spans="1:9" s="24" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A48" s="42"/>
-      <c r="B48" s="43"/>
-      <c r="C48" s="43"/>
+      <c r="A48" s="73"/>
+      <c r="B48" s="74"/>
+      <c r="C48" s="74"/>
       <c r="D48" s="23">
         <f>SUM(D16:D47)</f>
         <v>0.75</v>
       </c>
-      <c r="E48" s="44"/>
-      <c r="F48" s="44"/>
-      <c r="G48" s="44"/>
-      <c r="H48" s="44"/>
-      <c r="I48" s="45"/>
+      <c r="E48" s="75"/>
+      <c r="F48" s="75"/>
+      <c r="G48" s="75"/>
+      <c r="H48" s="75"/>
+      <c r="I48" s="76"/>
     </row>
     <row r="49" spans="1:12" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="18"/>
@@ -4071,16 +4064,33 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="E48:I48"/>
+    <mergeCell ref="E45:I45"/>
+    <mergeCell ref="E46:I46"/>
+    <mergeCell ref="E47:I47"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:I15"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="E44:I44"/>
+    <mergeCell ref="E39:I39"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="E41:I41"/>
+    <mergeCell ref="E36:I36"/>
+    <mergeCell ref="E37:I37"/>
+    <mergeCell ref="E38:I38"/>
+    <mergeCell ref="E34:I34"/>
+    <mergeCell ref="E35:I35"/>
+    <mergeCell ref="E30:I30"/>
+    <mergeCell ref="E31:I31"/>
+    <mergeCell ref="E32:I32"/>
     <mergeCell ref="E21:I21"/>
     <mergeCell ref="E22:I22"/>
     <mergeCell ref="E23:I23"/>
@@ -4097,33 +4107,16 @@
     <mergeCell ref="E25:I25"/>
     <mergeCell ref="E26:I26"/>
     <mergeCell ref="E33:I33"/>
-    <mergeCell ref="E34:I34"/>
-    <mergeCell ref="E35:I35"/>
-    <mergeCell ref="E30:I30"/>
-    <mergeCell ref="E31:I31"/>
-    <mergeCell ref="E32:I32"/>
-    <mergeCell ref="E39:I39"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="E41:I41"/>
-    <mergeCell ref="E36:I36"/>
-    <mergeCell ref="E37:I37"/>
-    <mergeCell ref="E38:I38"/>
-    <mergeCell ref="E48:I48"/>
-    <mergeCell ref="E45:I45"/>
-    <mergeCell ref="E46:I46"/>
-    <mergeCell ref="E47:I47"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:I15"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="E44:I44"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:H5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.44" right="0.03" top="0.02" bottom="0.03" header="0.19685039370078741" footer="0.19685039370078741"/>
@@ -4139,8 +4132,8 @@
   </sheetPr>
   <dimension ref="A1:AM49"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="110" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" zoomScalePageLayoutView="55" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24:I24"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A20" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47:I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -4158,18 +4151,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" s="6" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="72" t="str">
+      <c r="A1" s="36" t="str">
         <f>October!A1</f>
         <v>Monthly timesheet for MSc Geoinformatics ip:sdi - 23W856162</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -4202,126 +4195,126 @@
       <c r="AM1" s="1"/>
     </row>
     <row r="2" spans="1:39" s="1" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="73"/>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
     </row>
     <row r="3" spans="1:39" s="7" customFormat="1" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
       <c r="I3" s="14"/>
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
     </row>
     <row r="4" spans="1:39" s="1" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="75"/>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:39" s="1" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="64" t="str">
+      <c r="A5" s="42" t="str">
         <f>October!A5</f>
         <v>Firstname Lastname</v>
       </c>
-      <c r="B5" s="65"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="66" t="str">
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="44" t="str">
         <f>October!D5</f>
         <v>Stamatina Tounta</v>
       </c>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="68"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="46"/>
       <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:39" s="1" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="69"/>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="69"/>
-      <c r="H6" s="69"/>
-      <c r="I6" s="69"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
     </row>
     <row r="7" spans="1:39" s="1" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="70" t="str">
+      <c r="A7" s="48" t="str">
         <f>October!A7</f>
         <v>Project Acronym</v>
       </c>
-      <c r="B7" s="70"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="71" t="str">
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="49" t="str">
         <f>October!D7</f>
         <v>SudMig</v>
       </c>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
       <c r="I7" s="15"/>
     </row>
     <row r="8" spans="1:39" s="1" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="76"/>
-      <c r="B8" s="76"/>
-      <c r="C8" s="76"/>
-      <c r="D8" s="76"/>
-      <c r="E8" s="76"/>
-      <c r="F8" s="76"/>
-      <c r="G8" s="76"/>
-      <c r="H8" s="76"/>
-      <c r="I8" s="76"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
     </row>
     <row r="9" spans="1:39" s="1" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="70" t="str">
+      <c r="A9" s="48" t="str">
         <f>October!A9</f>
         <v>Project Title</v>
       </c>
-      <c r="B9" s="70"/>
-      <c r="C9" s="70"/>
-      <c r="D9" s="66" t="str">
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="44" t="str">
         <f>October!D9</f>
         <v>Sudan: monitoring migrant movements related to the 2023 conflict</v>
       </c>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="68"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="46"/>
       <c r="I9" s="15"/>
       <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:39" s="1" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="63"/>
-      <c r="B10" s="63"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="63"/>
+      <c r="A10" s="41"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
     </row>
     <row r="11" spans="1:39" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
@@ -4351,51 +4344,51 @@
       <c r="I12" s="16"/>
     </row>
     <row r="13" spans="1:39" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="50" t="s">
+      <c r="B13" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="52"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="55"/>
     </row>
     <row r="14" spans="1:39" s="2" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="48"/>
-      <c r="B14" s="53" t="s">
+      <c r="A14" s="51"/>
+      <c r="B14" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="54"/>
-      <c r="D14" s="55" t="s">
+      <c r="C14" s="57"/>
+      <c r="D14" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="57" t="s">
+      <c r="E14" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="58"/>
-      <c r="G14" s="58"/>
-      <c r="H14" s="58"/>
-      <c r="I14" s="59"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="62"/>
     </row>
     <row r="15" spans="1:39" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="49"/>
+      <c r="A15" s="52"/>
       <c r="B15" s="21" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="56"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
-      <c r="H15" s="61"/>
-      <c r="I15" s="62"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="64"/>
+      <c r="I15" s="65"/>
     </row>
     <row r="16" spans="1:39" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
@@ -4407,11 +4400,11 @@
         <f>C16-B16</f>
         <v>0</v>
       </c>
-      <c r="E16" s="39"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="41"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="70"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="71"/>
     </row>
     <row r="17" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="79" t="s">
@@ -4427,13 +4420,13 @@
         <f>C17-B17</f>
         <v>8.333333333333337E-2</v>
       </c>
-      <c r="E17" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="41"/>
+      <c r="E17" s="69" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="70"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="70"/>
+      <c r="I17" s="71"/>
     </row>
     <row r="18" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="80"/>
@@ -4447,13 +4440,13 @@
         <f t="shared" ref="D18:D47" si="0">C18-B18</f>
         <v>8.3333333333333259E-2</v>
       </c>
-      <c r="E18" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="38"/>
+      <c r="E18" s="66" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="68"/>
     </row>
     <row r="19" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="81"/>
@@ -4467,13 +4460,13 @@
         <f t="shared" si="0"/>
         <v>4.166666666666663E-2</v>
       </c>
-      <c r="E19" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="38"/>
+      <c r="E19" s="66" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="68"/>
     </row>
     <row r="20" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
@@ -4485,11 +4478,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E20" s="36"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="38"/>
+      <c r="E20" s="66"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="68"/>
     </row>
     <row r="21" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
@@ -4505,13 +4498,13 @@
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="E21" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="41"/>
+      <c r="E21" s="69" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" s="70"/>
+      <c r="G21" s="70"/>
+      <c r="H21" s="70"/>
+      <c r="I21" s="71"/>
     </row>
     <row r="22" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
@@ -4527,13 +4520,13 @@
         <f t="shared" si="0"/>
         <v>0.14583333333333337</v>
       </c>
-      <c r="E22" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="41"/>
+      <c r="E22" s="69" t="s">
+        <v>80</v>
+      </c>
+      <c r="F22" s="70"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="71"/>
     </row>
     <row r="23" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
@@ -4549,13 +4542,13 @@
         <f t="shared" si="0"/>
         <v>4.1666666666666741E-2</v>
       </c>
-      <c r="E23" s="39" t="s">
+      <c r="E23" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="41"/>
+      <c r="F23" s="70"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="70"/>
+      <c r="I23" s="71"/>
     </row>
     <row r="24" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
@@ -4567,11 +4560,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E24" s="39"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="41"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="70"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="70"/>
+      <c r="I24" s="71"/>
     </row>
     <row r="25" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
@@ -4583,11 +4576,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E25" s="39"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="41"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="70"/>
+      <c r="G25" s="70"/>
+      <c r="H25" s="70"/>
+      <c r="I25" s="71"/>
     </row>
     <row r="26" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
@@ -4599,43 +4592,55 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E26" s="36"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="38"/>
+      <c r="E26" s="66"/>
+      <c r="F26" s="67"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="67"/>
+      <c r="I26" s="68"/>
     </row>
     <row r="27" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="27"/>
+      <c r="B27" s="26">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C27" s="27">
+        <v>0.85416666666666663</v>
+      </c>
       <c r="D27" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E27" s="36"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="38"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="E27" s="66" t="s">
+        <v>82</v>
+      </c>
+      <c r="F27" s="67"/>
+      <c r="G27" s="67"/>
+      <c r="H27" s="67"/>
+      <c r="I27" s="68"/>
     </row>
     <row r="28" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="31"/>
+      <c r="B28" s="30">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C28" s="31">
+        <v>0.75</v>
+      </c>
       <c r="D28" s="31">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E28" s="39"/>
-      <c r="F28" s="40"/>
-      <c r="G28" s="40"/>
-      <c r="H28" s="40"/>
-      <c r="I28" s="41"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E28" s="69" t="s">
+        <v>83</v>
+      </c>
+      <c r="F28" s="70"/>
+      <c r="G28" s="70"/>
+      <c r="H28" s="70"/>
+      <c r="I28" s="71"/>
     </row>
     <row r="29" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="29" t="s">
@@ -4647,11 +4652,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E29" s="39"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="41"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="70"/>
+      <c r="G29" s="70"/>
+      <c r="H29" s="70"/>
+      <c r="I29" s="71"/>
     </row>
     <row r="30" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="29" t="s">
@@ -4663,11 +4668,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E30" s="39"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="41"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="70"/>
+      <c r="G30" s="70"/>
+      <c r="H30" s="70"/>
+      <c r="I30" s="71"/>
     </row>
     <row r="31" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
@@ -4679,11 +4684,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E31" s="39"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="41"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="70"/>
+      <c r="I31" s="71"/>
     </row>
     <row r="32" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="29" t="s">
@@ -4695,27 +4700,33 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E32" s="39"/>
-      <c r="F32" s="40"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="40"/>
-      <c r="I32" s="41"/>
+      <c r="E32" s="69"/>
+      <c r="F32" s="70"/>
+      <c r="G32" s="70"/>
+      <c r="H32" s="70"/>
+      <c r="I32" s="71"/>
     </row>
     <row r="33" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="26"/>
-      <c r="C33" s="27"/>
+      <c r="B33" s="26">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C33" s="27">
+        <v>0.5</v>
+      </c>
       <c r="D33" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E33" s="36"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="38"/>
+        <v>0.10416666666666669</v>
+      </c>
+      <c r="E33" s="66" t="s">
+        <v>84</v>
+      </c>
+      <c r="F33" s="67"/>
+      <c r="G33" s="67"/>
+      <c r="H33" s="67"/>
+      <c r="I33" s="68"/>
     </row>
     <row r="34" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
@@ -4727,11 +4738,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E34" s="36"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="37"/>
-      <c r="H34" s="37"/>
-      <c r="I34" s="38"/>
+      <c r="E34" s="66"/>
+      <c r="F34" s="67"/>
+      <c r="G34" s="67"/>
+      <c r="H34" s="67"/>
+      <c r="I34" s="68"/>
     </row>
     <row r="35" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="29" t="s">
@@ -4743,43 +4754,55 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E35" s="39"/>
-      <c r="F35" s="40"/>
-      <c r="G35" s="40"/>
-      <c r="H35" s="40"/>
-      <c r="I35" s="41"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="70"/>
+      <c r="H35" s="70"/>
+      <c r="I35" s="71"/>
     </row>
     <row r="36" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="30"/>
-      <c r="C36" s="31"/>
+      <c r="B36" s="30">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C36" s="31">
+        <v>0.77083333333333337</v>
+      </c>
       <c r="D36" s="31">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="40"/>
-      <c r="G36" s="40"/>
-      <c r="H36" s="40"/>
-      <c r="I36" s="41"/>
+        <v>0.125</v>
+      </c>
+      <c r="E36" s="69" t="s">
+        <v>85</v>
+      </c>
+      <c r="F36" s="70"/>
+      <c r="G36" s="70"/>
+      <c r="H36" s="70"/>
+      <c r="I36" s="71"/>
     </row>
     <row r="37" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="30"/>
-      <c r="C37" s="31"/>
+      <c r="B37" s="30">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C37" s="31">
+        <v>0.75</v>
+      </c>
       <c r="D37" s="31">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="40"/>
-      <c r="G37" s="40"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="41"/>
+        <v>0.10416666666666663</v>
+      </c>
+      <c r="E37" s="69" t="s">
+        <v>86</v>
+      </c>
+      <c r="F37" s="70"/>
+      <c r="G37" s="70"/>
+      <c r="H37" s="70"/>
+      <c r="I37" s="71"/>
     </row>
     <row r="38" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="29" t="s">
@@ -4791,11 +4814,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E38" s="39"/>
-      <c r="F38" s="40"/>
-      <c r="G38" s="40"/>
-      <c r="H38" s="40"/>
-      <c r="I38" s="41"/>
+      <c r="E38" s="69"/>
+      <c r="F38" s="70"/>
+      <c r="G38" s="70"/>
+      <c r="H38" s="70"/>
+      <c r="I38" s="71"/>
     </row>
     <row r="39" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="29" t="s">
@@ -4807,43 +4830,55 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E39" s="39"/>
-      <c r="F39" s="40"/>
-      <c r="G39" s="40"/>
-      <c r="H39" s="40"/>
-      <c r="I39" s="41"/>
+      <c r="E39" s="69"/>
+      <c r="F39" s="70"/>
+      <c r="G39" s="70"/>
+      <c r="H39" s="70"/>
+      <c r="I39" s="71"/>
     </row>
     <row r="40" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="26"/>
-      <c r="C40" s="27"/>
+      <c r="B40" s="26">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C40" s="27">
+        <v>0.5</v>
+      </c>
       <c r="D40" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E40" s="36"/>
-      <c r="F40" s="37"/>
-      <c r="G40" s="37"/>
-      <c r="H40" s="37"/>
-      <c r="I40" s="38"/>
+        <v>8.3333333333333315E-2</v>
+      </c>
+      <c r="E40" s="66" t="s">
+        <v>89</v>
+      </c>
+      <c r="F40" s="67"/>
+      <c r="G40" s="67"/>
+      <c r="H40" s="67"/>
+      <c r="I40" s="68"/>
     </row>
     <row r="41" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="B41" s="26"/>
-      <c r="C41" s="27"/>
+      <c r="B41" s="26">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C41" s="27">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="D41" s="27">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E41" s="36"/>
-      <c r="F41" s="37"/>
-      <c r="G41" s="37"/>
-      <c r="H41" s="37"/>
-      <c r="I41" s="38"/>
+        <v>8.3333333333333259E-2</v>
+      </c>
+      <c r="E41" s="66" t="s">
+        <v>87</v>
+      </c>
+      <c r="F41" s="67"/>
+      <c r="G41" s="67"/>
+      <c r="H41" s="67"/>
+      <c r="I41" s="68"/>
     </row>
     <row r="42" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="29" t="s">
@@ -4855,11 +4890,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E42" s="39"/>
-      <c r="F42" s="40"/>
-      <c r="G42" s="40"/>
-      <c r="H42" s="40"/>
-      <c r="I42" s="41"/>
+      <c r="E42" s="69"/>
+      <c r="F42" s="70"/>
+      <c r="G42" s="70"/>
+      <c r="H42" s="70"/>
+      <c r="I42" s="71"/>
     </row>
     <row r="43" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="29" t="s">
@@ -4871,11 +4906,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E43" s="39"/>
-      <c r="F43" s="40"/>
-      <c r="G43" s="40"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="41"/>
+      <c r="E43" s="69"/>
+      <c r="F43" s="70"/>
+      <c r="G43" s="70"/>
+      <c r="H43" s="70"/>
+      <c r="I43" s="71"/>
     </row>
     <row r="44" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="29" t="s">
@@ -4887,43 +4922,55 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E44" s="39"/>
-      <c r="F44" s="40"/>
-      <c r="G44" s="40"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="41"/>
+      <c r="E44" s="69"/>
+      <c r="F44" s="70"/>
+      <c r="G44" s="70"/>
+      <c r="H44" s="70"/>
+      <c r="I44" s="71"/>
     </row>
     <row r="45" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="30"/>
-      <c r="C45" s="31"/>
+      <c r="B45" s="30">
+        <v>0.75</v>
+      </c>
+      <c r="C45" s="31">
+        <v>0.83333333333333337</v>
+      </c>
       <c r="D45" s="31">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E45" s="39"/>
-      <c r="F45" s="40"/>
-      <c r="G45" s="40"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="41"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E45" s="69" t="s">
+        <v>88</v>
+      </c>
+      <c r="F45" s="70"/>
+      <c r="G45" s="70"/>
+      <c r="H45" s="70"/>
+      <c r="I45" s="71"/>
     </row>
     <row r="46" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="30"/>
-      <c r="C46" s="31"/>
+      <c r="B46" s="30">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C46" s="31">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="D46" s="31">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E46" s="39"/>
-      <c r="F46" s="40"/>
-      <c r="G46" s="40"/>
-      <c r="H46" s="40"/>
-      <c r="I46" s="41"/>
+        <v>0.125</v>
+      </c>
+      <c r="E46" s="69" t="s">
+        <v>90</v>
+      </c>
+      <c r="F46" s="70"/>
+      <c r="G46" s="70"/>
+      <c r="H46" s="70"/>
+      <c r="I46" s="71"/>
     </row>
     <row r="47" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="25" t="s">
@@ -4935,25 +4982,25 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E47" s="36"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="37"/>
-      <c r="H47" s="37"/>
-      <c r="I47" s="38"/>
+      <c r="E47" s="66"/>
+      <c r="F47" s="67"/>
+      <c r="G47" s="67"/>
+      <c r="H47" s="67"/>
+      <c r="I47" s="68"/>
     </row>
     <row r="48" spans="1:9" s="24" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A48" s="42"/>
-      <c r="B48" s="43"/>
-      <c r="C48" s="43"/>
+      <c r="A48" s="73"/>
+      <c r="B48" s="74"/>
+      <c r="C48" s="74"/>
       <c r="D48" s="23">
         <f>SUM(D16:D47)</f>
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="E48" s="44"/>
-      <c r="F48" s="44"/>
-      <c r="G48" s="44"/>
-      <c r="H48" s="44"/>
-      <c r="I48" s="45"/>
+        <v>1.5</v>
+      </c>
+      <c r="E48" s="75"/>
+      <c r="F48" s="75"/>
+      <c r="G48" s="75"/>
+      <c r="H48" s="75"/>
+      <c r="I48" s="76"/>
     </row>
     <row r="49" spans="1:12" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="18"/>
@@ -4971,32 +5018,27 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:H7"/>
-    <mergeCell ref="A8:I8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:I15"/>
+    <mergeCell ref="E41:I41"/>
+    <mergeCell ref="E30:I30"/>
+    <mergeCell ref="E31:I31"/>
+    <mergeCell ref="E32:I32"/>
+    <mergeCell ref="E33:I33"/>
+    <mergeCell ref="E36:I36"/>
+    <mergeCell ref="E37:I37"/>
+    <mergeCell ref="E38:I38"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="E48:I48"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="E44:I44"/>
+    <mergeCell ref="E45:I45"/>
+    <mergeCell ref="E46:I46"/>
+    <mergeCell ref="E47:I47"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="E19:I19"/>
     <mergeCell ref="E39:I39"/>
     <mergeCell ref="E40:I40"/>
     <mergeCell ref="E29:I29"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="E21:I21"/>
-    <mergeCell ref="E22:I22"/>
     <mergeCell ref="E23:I23"/>
     <mergeCell ref="E24:I24"/>
     <mergeCell ref="E25:I25"/>
@@ -5005,25 +5047,30 @@
     <mergeCell ref="E28:I28"/>
     <mergeCell ref="E34:I34"/>
     <mergeCell ref="E35:I35"/>
-    <mergeCell ref="E36:I36"/>
-    <mergeCell ref="E37:I37"/>
-    <mergeCell ref="E38:I38"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
     <mergeCell ref="E17:I17"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="E19:I19"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="E48:I48"/>
-    <mergeCell ref="E42:I42"/>
-    <mergeCell ref="E43:I43"/>
-    <mergeCell ref="E44:I44"/>
-    <mergeCell ref="E45:I45"/>
-    <mergeCell ref="E46:I46"/>
-    <mergeCell ref="E47:I47"/>
-    <mergeCell ref="E41:I41"/>
-    <mergeCell ref="E30:I30"/>
-    <mergeCell ref="E31:I31"/>
-    <mergeCell ref="E32:I32"/>
-    <mergeCell ref="E33:I33"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:I15"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:H5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.44" right="0.03" top="0.02" bottom="0.03" header="0.19685039370078741" footer="0.19685039370078741"/>
@@ -5033,15 +5080,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E194172A664C3D44B55AD259CF5259CC" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="465a3c731076d5a6b41531443f0de4f6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="efe5fd09-895f-413c-ad62-8a7b7313e3f2" xmlns:ns3="34840fcf-b2b1-4e6c-965a-1d79bbd7ca53" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d8e2dec1e433440d6e71b07ff70d1d2a" ns2:_="" ns3:_="">
     <xsd:import namespace="efe5fd09-895f-413c-ad62-8a7b7313e3f2"/>
@@ -5212,15 +5250,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB82E1FC-3531-46DB-87B4-2724210208FD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{932AD44C-3965-4F84-937C-EB34F79113F9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5237,4 +5276,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB82E1FC-3531-46DB-87B4-2724210208FD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Uploading most up-to-date timesheet. Replace ip_sdi_time_sheet_s1095334.xlsx
</commit_message>
<xml_diff>
--- a/Project_management/ip_sdi_time_sheet_s1095334.xlsx
+++ b/Project_management/ip_sdi_time_sheet_s1095334.xlsx
@@ -8,24 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://plusacat-my.sharepoint.com/personal/stamatina_tounta_stud_plus_ac_at/Documents/3rd semester/IP_SDI/4. Project/3. Project management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="138" documentId="13_ncr:1_{70D4A704-C547-4687-9C54-B5A46D362BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01B03708-8C5C-45E0-B7A6-48E6022678F6}"/>
+  <xr:revisionPtr revIDLastSave="166" documentId="13_ncr:1_{70D4A704-C547-4687-9C54-B5A46D362BE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D55D4D6-B0C3-4EF6-AF64-7BA6E31E2D4F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="893" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="893" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="October" sheetId="7" r:id="rId1"/>
     <sheet name="November" sheetId="4" r:id="rId2"/>
     <sheet name="December" sheetId="5" r:id="rId3"/>
     <sheet name="January" sheetId="13" r:id="rId4"/>
+    <sheet name="February" sheetId="14" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="E_satz">#REF!</definedName>
     <definedName name="M_satz">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">December!$A$1:$L$49</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">February!$A$1:$L$49</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">January!$A$1:$L$49</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">November!$A$1:$L$47</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">October!$A$1:$I$48</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">December!$16:$18</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="4">February!$16:$18</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">January!$16:$18</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">November!$16:$17</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">October!$13:$15</definedName>
@@ -54,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="96">
   <si>
     <t>Monthly timesheet for MSc Geoinformatics ip:sdi - 23W856162</t>
   </si>
@@ -337,6 +340,21 @@
   </si>
   <si>
     <t>Team meeting: finalizing ArcGIS Insights (WP4) and final presentation (WP0)/ preparing for the presentation (WP0)</t>
+  </si>
+  <si>
+    <t>Updating GitLab Wiki (WP0)</t>
+  </si>
+  <si>
+    <t>Start updating project report (WP0)</t>
+  </si>
+  <si>
+    <t>Project report update (WP0)</t>
+  </si>
+  <si>
+    <t>Group meeting: GitLab and project report status/ Working on project report (WP0)</t>
+  </si>
+  <si>
+    <t>Finalizing project report (WP0)</t>
   </si>
 </sst>
 </file>
@@ -3212,7 +3230,7 @@
   </sheetPr>
   <dimension ref="A1:AM49"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A27" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="E47" sqref="E47:I47"/>
     </sheetView>
   </sheetViews>
@@ -4132,7 +4150,7 @@
   </sheetPr>
   <dimension ref="A1:AM49"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A20" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="55" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A33" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="55" workbookViewId="0">
       <selection activeCell="E47" sqref="E47:I47"/>
     </sheetView>
   </sheetViews>
@@ -5079,7 +5097,916 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F31472-33F4-478C-96A4-2FF929F614E7}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:AM49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A14" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34:I34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="3" width="5.5546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="3.44140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="38.88671875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="7.5546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="3.109375" style="3" customWidth="1"/>
+    <col min="10" max="12" width="11.44140625" style="3" hidden="1" customWidth="1"/>
+    <col min="13" max="256" width="11.44140625" style="3" customWidth="1"/>
+    <col min="257" max="16384" width="9.109375" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:39" s="6" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="str">
+        <f>October!A1</f>
+        <v>Monthly timesheet for MSc Geoinformatics ip:sdi - 23W856162</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="1"/>
+      <c r="AM1" s="1"/>
+    </row>
+    <row r="2" spans="1:39" s="1" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+    </row>
+    <row r="3" spans="1:39" s="7" customFormat="1" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+    </row>
+    <row r="4" spans="1:39" s="1" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+    </row>
+    <row r="5" spans="1:39" s="1" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="42" t="str">
+        <f>October!A5</f>
+        <v>Firstname Lastname</v>
+      </c>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="44" t="str">
+        <f>October!D5</f>
+        <v>Stamatina Tounta</v>
+      </c>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="14"/>
+    </row>
+    <row r="6" spans="1:39" s="1" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="47"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+    </row>
+    <row r="7" spans="1:39" s="1" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="48" t="str">
+        <f>October!A7</f>
+        <v>Project Acronym</v>
+      </c>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="49" t="str">
+        <f>October!D7</f>
+        <v>SudMig</v>
+      </c>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="15"/>
+    </row>
+    <row r="8" spans="1:39" s="1" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+    </row>
+    <row r="9" spans="1:39" s="1" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="48" t="str">
+        <f>October!A9</f>
+        <v>Project Title</v>
+      </c>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="44" t="str">
+        <f>October!D9</f>
+        <v>Sudan: monitoring migrant movements related to the 2023 conflict</v>
+      </c>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:39" s="1" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="41"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+    </row>
+    <row r="11" spans="1:39" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A11" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34" t="str">
+        <f>October!D11</f>
+        <v>Winter Term 2023 / 2024</v>
+      </c>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="14"/>
+    </row>
+    <row r="12" spans="1:39" s="1" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+    </row>
+    <row r="13" spans="1:39" s="2" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="55"/>
+    </row>
+    <row r="14" spans="1:39" s="2" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="51"/>
+      <c r="B14" s="56" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="57"/>
+      <c r="D14" s="58" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="62"/>
+    </row>
+    <row r="15" spans="1:39" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="52"/>
+      <c r="B15" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="59"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="64"/>
+      <c r="I15" s="65"/>
+    </row>
+    <row r="16" spans="1:39" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="30"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31">
+        <f>C16-B16</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="69"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="70"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="71"/>
+    </row>
+    <row r="17" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A17" s="79" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="30"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31">
+        <f>C17-B17</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="69"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="70"/>
+      <c r="I17" s="71"/>
+    </row>
+    <row r="18" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A18" s="80"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27">
+        <f t="shared" ref="D18:D47" si="0">C18-B18</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="66"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="68"/>
+    </row>
+    <row r="19" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A19" s="81"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E19" s="66"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="68"/>
+    </row>
+    <row r="20" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="26"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="66"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="68"/>
+    </row>
+    <row r="21" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="30"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E21" s="69"/>
+      <c r="F21" s="70"/>
+      <c r="G21" s="70"/>
+      <c r="H21" s="70"/>
+      <c r="I21" s="71"/>
+    </row>
+    <row r="22" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A22" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="30">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C22" s="31">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D22" s="31">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+      <c r="E22" s="69" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" s="70"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="71"/>
+    </row>
+    <row r="23" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A23" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="30"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E23" s="69"/>
+      <c r="F23" s="70"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="70"/>
+      <c r="I23" s="71"/>
+    </row>
+    <row r="24" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A24" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="30"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E24" s="69"/>
+      <c r="F24" s="70"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="70"/>
+      <c r="I24" s="71"/>
+    </row>
+    <row r="25" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A25" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="30">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C25" s="31">
+        <v>0.75</v>
+      </c>
+      <c r="D25" s="31">
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E25" s="69" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="70"/>
+      <c r="G25" s="70"/>
+      <c r="H25" s="70"/>
+      <c r="I25" s="71"/>
+    </row>
+    <row r="26" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A26" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="26"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E26" s="66"/>
+      <c r="F26" s="67"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="67"/>
+      <c r="I26" s="68"/>
+    </row>
+    <row r="27" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A27" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="26">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C27" s="27">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D27" s="27">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333315E-2</v>
+      </c>
+      <c r="E27" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="F27" s="67"/>
+      <c r="G27" s="67"/>
+      <c r="H27" s="67"/>
+      <c r="I27" s="68"/>
+    </row>
+    <row r="28" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A28" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="30"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E28" s="69"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="70"/>
+      <c r="H28" s="70"/>
+      <c r="I28" s="71"/>
+    </row>
+    <row r="29" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A29" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="30"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E29" s="69"/>
+      <c r="F29" s="70"/>
+      <c r="G29" s="70"/>
+      <c r="H29" s="70"/>
+      <c r="I29" s="71"/>
+    </row>
+    <row r="30" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A30" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="30"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E30" s="69"/>
+      <c r="F30" s="70"/>
+      <c r="G30" s="70"/>
+      <c r="H30" s="70"/>
+      <c r="I30" s="71"/>
+    </row>
+    <row r="31" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A31" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="30">
+        <v>0.75</v>
+      </c>
+      <c r="C31" s="31">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D31" s="31">
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E31" s="69" t="s">
+        <v>93</v>
+      </c>
+      <c r="F31" s="70"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="70"/>
+      <c r="I31" s="71"/>
+    </row>
+    <row r="32" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A32" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="30"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E32" s="69"/>
+      <c r="F32" s="70"/>
+      <c r="G32" s="70"/>
+      <c r="H32" s="70"/>
+      <c r="I32" s="71"/>
+    </row>
+    <row r="33" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A33" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="26">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C33" s="27">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D33" s="27">
+        <f t="shared" si="0"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="E33" s="66" t="s">
+        <v>94</v>
+      </c>
+      <c r="F33" s="67"/>
+      <c r="G33" s="67"/>
+      <c r="H33" s="67"/>
+      <c r="I33" s="68"/>
+    </row>
+    <row r="34" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A34" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="C34" s="27">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D34" s="27">
+        <f t="shared" si="0"/>
+        <v>0.10416666666666663</v>
+      </c>
+      <c r="E34" s="66" t="s">
+        <v>95</v>
+      </c>
+      <c r="F34" s="67"/>
+      <c r="G34" s="67"/>
+      <c r="H34" s="67"/>
+      <c r="I34" s="68"/>
+    </row>
+    <row r="35" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A35" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="30"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E35" s="69"/>
+      <c r="F35" s="70"/>
+      <c r="G35" s="70"/>
+      <c r="H35" s="70"/>
+      <c r="I35" s="71"/>
+    </row>
+    <row r="36" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A36" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="30"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E36" s="69"/>
+      <c r="F36" s="70"/>
+      <c r="G36" s="70"/>
+      <c r="H36" s="70"/>
+      <c r="I36" s="71"/>
+    </row>
+    <row r="37" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A37" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="30"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E37" s="69"/>
+      <c r="F37" s="70"/>
+      <c r="G37" s="70"/>
+      <c r="H37" s="70"/>
+      <c r="I37" s="71"/>
+    </row>
+    <row r="38" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A38" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="30"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E38" s="69"/>
+      <c r="F38" s="70"/>
+      <c r="G38" s="70"/>
+      <c r="H38" s="70"/>
+      <c r="I38" s="71"/>
+    </row>
+    <row r="39" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A39" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="30"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E39" s="69"/>
+      <c r="F39" s="70"/>
+      <c r="G39" s="70"/>
+      <c r="H39" s="70"/>
+      <c r="I39" s="71"/>
+    </row>
+    <row r="40" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A40" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B40" s="26"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E40" s="66"/>
+      <c r="F40" s="67"/>
+      <c r="G40" s="67"/>
+      <c r="H40" s="67"/>
+      <c r="I40" s="68"/>
+    </row>
+    <row r="41" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A41" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="26"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E41" s="66"/>
+      <c r="F41" s="67"/>
+      <c r="G41" s="67"/>
+      <c r="H41" s="67"/>
+      <c r="I41" s="68"/>
+    </row>
+    <row r="42" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A42" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" s="30"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E42" s="69"/>
+      <c r="F42" s="70"/>
+      <c r="G42" s="70"/>
+      <c r="H42" s="70"/>
+      <c r="I42" s="71"/>
+    </row>
+    <row r="43" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A43" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" s="30"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E43" s="69"/>
+      <c r="F43" s="70"/>
+      <c r="G43" s="70"/>
+      <c r="H43" s="70"/>
+      <c r="I43" s="71"/>
+    </row>
+    <row r="44" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A44" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B44" s="30"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E44" s="69"/>
+      <c r="F44" s="70"/>
+      <c r="G44" s="70"/>
+      <c r="H44" s="70"/>
+      <c r="I44" s="71"/>
+    </row>
+    <row r="45" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A45" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" s="30"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E45" s="69"/>
+      <c r="F45" s="70"/>
+      <c r="G45" s="70"/>
+      <c r="H45" s="70"/>
+      <c r="I45" s="71"/>
+    </row>
+    <row r="46" spans="1:9" s="32" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A46" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" s="30"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E46" s="69"/>
+      <c r="F46" s="70"/>
+      <c r="G46" s="70"/>
+      <c r="H46" s="70"/>
+      <c r="I46" s="71"/>
+    </row>
+    <row r="47" spans="1:9" s="28" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A47" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47" s="26"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E47" s="66"/>
+      <c r="F47" s="67"/>
+      <c r="G47" s="67"/>
+      <c r="H47" s="67"/>
+      <c r="I47" s="68"/>
+    </row>
+    <row r="48" spans="1:9" s="24" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A48" s="73"/>
+      <c r="B48" s="74"/>
+      <c r="C48" s="74"/>
+      <c r="D48" s="23">
+        <f>SUM(D16:D47)</f>
+        <v>0.5625</v>
+      </c>
+      <c r="E48" s="75"/>
+      <c r="F48" s="75"/>
+      <c r="G48" s="75"/>
+      <c r="H48" s="75"/>
+      <c r="I48" s="76"/>
+    </row>
+    <row r="49" spans="1:12" ht="7.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="18"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="18"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="9"/>
+      <c r="K49" s="9"/>
+      <c r="L49" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="53">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:H7"/>
+    <mergeCell ref="A8:I8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:I15"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="E19:I19"/>
+    <mergeCell ref="E32:I32"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E26:I26"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E28:I28"/>
+    <mergeCell ref="E29:I29"/>
+    <mergeCell ref="E30:I30"/>
+    <mergeCell ref="E31:I31"/>
+    <mergeCell ref="E44:I44"/>
+    <mergeCell ref="E33:I33"/>
+    <mergeCell ref="E34:I34"/>
+    <mergeCell ref="E35:I35"/>
+    <mergeCell ref="E36:I36"/>
+    <mergeCell ref="E37:I37"/>
+    <mergeCell ref="E38:I38"/>
+    <mergeCell ref="E39:I39"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="E41:I41"/>
+    <mergeCell ref="E42:I42"/>
+    <mergeCell ref="E43:I43"/>
+    <mergeCell ref="E45:I45"/>
+    <mergeCell ref="E46:I46"/>
+    <mergeCell ref="E47:I47"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="E48:I48"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.44" right="0.03" top="0.02" bottom="0.03" header="0.19685039370078741" footer="0.19685039370078741"/>
+  <pageSetup paperSize="9" scale="95" orientation="landscape" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E194172A664C3D44B55AD259CF5259CC" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="465a3c731076d5a6b41531443f0de4f6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="efe5fd09-895f-413c-ad62-8a7b7313e3f2" xmlns:ns3="34840fcf-b2b1-4e6c-965a-1d79bbd7ca53" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d8e2dec1e433440d6e71b07ff70d1d2a" ns2:_="" ns3:_="">
     <xsd:import namespace="efe5fd09-895f-413c-ad62-8a7b7313e3f2"/>
@@ -5250,16 +6177,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB82E1FC-3531-46DB-87B4-2724210208FD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{932AD44C-3965-4F84-937C-EB34F79113F9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5276,12 +6202,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB82E1FC-3531-46DB-87B4-2724210208FD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>